<commit_message>
Added function to identify deletions by low coverage only
This feature is not 100% complete yet
</commit_message>
<xml_diff>
--- a/LLStrains.xlsx
+++ b/LLStrains.xlsx
@@ -600,7 +600,7 @@
       </c>
       <c r="S4" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L adhE H734R Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T4" s="0" t="inlineStr">
@@ -1000,7 +1000,11 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="R13" s="0" t="inlineStr"/>
+      <c r="R13" s="0" t="inlineStr">
+        <is>
+          <t>Identical to LL345, as far as I can tell</t>
+        </is>
+      </c>
       <c r="S13" s="0" t="inlineStr">
         <is>
           <t> ∆hpt</t>
@@ -1080,7 +1084,7 @@
       </c>
       <c r="H15" s="0" t="inlineStr">
         <is>
-          <t>AG2061</t>
+          <t>AG1326</t>
         </is>
       </c>
       <c r="S15" s="0" t="inlineStr">
@@ -1125,7 +1129,6 @@
       <c r="E16" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F16" s="0" t="inlineStr"/>
       <c r="G16" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -1583,9 +1586,14 @@
           <t>AG599</t>
         </is>
       </c>
+      <c r="R26" s="0" t="inlineStr">
+        <is>
+          <t>ldh mutation is not automatically detected because there's an extra left BP that got annotated by CLC.</t>
+        </is>
+      </c>
       <c r="S26" s="0" t="inlineStr">
         <is>
-          <t> adhE D494G ∆hpt ∆hydG ∆pfl ∆(pta-ack) [adapted]</t>
+          <t> adhE D494G ∆hpt ∆hydG ∆ldh ∆pfl ∆(pta-ack) [adapted]</t>
         </is>
       </c>
       <c r="T26" s="0" t="inlineStr">
@@ -1768,7 +1776,7 @@
       </c>
       <c r="S30" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T30" s="0" t="inlineStr">
@@ -1810,7 +1818,7 @@
       </c>
       <c r="S31" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T31" s="0" t="inlineStr">
@@ -1852,7 +1860,7 @@
       </c>
       <c r="S32" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T32" s="0" t="inlineStr">
@@ -1882,7 +1890,6 @@
       <c r="E33" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F33" s="0" t="inlineStr"/>
       <c r="G33" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -1893,12 +1900,9 @@
           <t>LL1304</t>
         </is>
       </c>
-      <c r="I33" s="0" t="inlineStr"/>
-      <c r="P33" s="0" t="inlineStr"/>
-      <c r="R33" s="0" t="inlineStr"/>
       <c r="S33" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T33" s="0" t="inlineStr">
@@ -1912,7 +1916,6 @@
       <c r="U33" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="Y33" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="34">
       <c r="A34" s="0" t="inlineStr">
@@ -1929,7 +1932,6 @@
       <c r="E34" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F34" s="0" t="inlineStr"/>
       <c r="G34" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -1940,12 +1942,9 @@
           <t>LL1304</t>
         </is>
       </c>
-      <c r="I34" s="0" t="inlineStr"/>
-      <c r="P34" s="0" t="inlineStr"/>
-      <c r="R34" s="0" t="inlineStr"/>
       <c r="S34" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T34" s="0" t="inlineStr">
@@ -1959,7 +1958,6 @@
       <c r="U34" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="Y34" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="35">
       <c r="A35" s="0" t="inlineStr">
@@ -1976,7 +1974,6 @@
       <c r="E35" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F35" s="0" t="inlineStr"/>
       <c r="G35" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -1987,12 +1984,9 @@
           <t>LL1304</t>
         </is>
       </c>
-      <c r="I35" s="0" t="inlineStr"/>
-      <c r="P35" s="0" t="inlineStr"/>
-      <c r="R35" s="0" t="inlineStr"/>
       <c r="S35" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T35" s="0" t="inlineStr">
@@ -2006,7 +2000,6 @@
       <c r="U35" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="Y35" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="36">
       <c r="A36" s="0" t="inlineStr">
@@ -2023,7 +2016,6 @@
       <c r="E36" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F36" s="0" t="inlineStr"/>
       <c r="G36" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -2034,12 +2026,9 @@
           <t>LL1304</t>
         </is>
       </c>
-      <c r="I36" s="0" t="inlineStr"/>
-      <c r="P36" s="0" t="inlineStr"/>
-      <c r="R36" s="0" t="inlineStr"/>
       <c r="S36" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T36" s="0" t="inlineStr">
@@ -2053,7 +2042,6 @@
       <c r="U36" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="Y36" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="37">
       <c r="A37" s="0" t="inlineStr">
@@ -2067,11 +2055,9 @@
       <c r="C37" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D37" s="0" t="inlineStr"/>
       <c r="E37" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="0" t="inlineStr"/>
       <c r="G37" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -2082,15 +2068,9 @@
           <t>LL1304</t>
         </is>
       </c>
-      <c r="K37" s="0" t="inlineStr"/>
-      <c r="L37" s="0" t="inlineStr"/>
-      <c r="M37" s="0" t="inlineStr"/>
-      <c r="N37" s="0" t="inlineStr"/>
-      <c r="P37" s="0" t="inlineStr"/>
-      <c r="R37" s="0" t="inlineStr"/>
       <c r="S37" s="0" t="inlineStr">
         <is>
-          <t> Δhpt ∆ldh</t>
+          <t> adhE P704L Δhpt ∆ldh</t>
         </is>
       </c>
       <c r="T37" s="0" t="inlineStr">
@@ -2104,7 +2084,6 @@
       <c r="U37" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="Y37" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="38">
       <c r="A38" s="0" t="inlineStr">
@@ -2121,7 +2100,6 @@
       <c r="E38" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F38" s="0" t="inlineStr"/>
       <c r="G38" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -2132,12 +2110,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="K38" s="0" t="inlineStr"/>
-      <c r="L38" s="0" t="inlineStr"/>
-      <c r="M38" s="0" t="inlineStr"/>
-      <c r="N38" s="0" t="inlineStr"/>
-      <c r="Q38" s="0" t="inlineStr"/>
-      <c r="R38" s="0" t="inlineStr"/>
       <c r="S38" s="0" t="inlineStr">
         <is>
           <t> ∆hpt ΔreIII</t>
@@ -2153,7 +2125,6 @@
       <c r="U38" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="Y38" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="39">
       <c r="A39" s="0" t="inlineStr">
@@ -2170,7 +2141,6 @@
       <c r="E39" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F39" s="0" t="inlineStr"/>
       <c r="G39" s="0" t="inlineStr">
         <is>
           <t>Clostridium thermocellum</t>
@@ -2181,8 +2151,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="Q39" s="0" t="inlineStr"/>
-      <c r="R39" s="0" t="inlineStr"/>
       <c r="S39" s="0" t="inlineStr">
         <is>
           <t> ∆hpt Δre2366</t>
@@ -2198,7 +2166,6 @@
       <c r="U39" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="Y39" s="0" t="inlineStr"/>
     </row>
     <row outlineLevel="0" r="40">
       <c r="A40" s="0" t="inlineStr">
@@ -2397,7 +2364,6 @@
       <c r="C43" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D43" s="0" t="inlineStr"/>
       <c r="E43" s="0" t="b">
         <v>0</v>
       </c>
@@ -2431,7 +2397,6 @@
           <t>celY deletion strain</t>
         </is>
       </c>
-      <c r="S43" s="0" t="inlineStr"/>
       <c r="T43" s="0" t="inlineStr">
         <is>
           <t>LL1005 _x000d_
@@ -2478,7 +2443,6 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="H44" s="0" t="inlineStr"/>
       <c r="K44" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -2509,8 +2473,6 @@
           <t>Clostridium thermocellum DSM1313, 1st generation stock made from DSMZ lyophylized vial, wild type, M0003, DS1, WT, 1313</t>
         </is>
       </c>
-      <c r="S44" s="0" t="inlineStr"/>
-      <c r="T44" s="0" t="inlineStr"/>
       <c r="U44" s="0" t="b">
         <v>0</v>
       </c>
@@ -2950,13 +2912,11 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="H52" s="0" t="inlineStr"/>
       <c r="R52" s="0" t="inlineStr">
         <is>
           <t>DS10, M41, M0041, ATCC 27405, Clostridium thermocellum ATCC 27405, 1st generation stock from ATCC culture</t>
         </is>
       </c>
-      <c r="T52" s="0" t="inlineStr"/>
       <c r="U52" s="0" t="b">
         <v>0</v>
       </c>
@@ -3103,10 +3063,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="K55" s="0" t="inlineStr"/>
-      <c r="L55" s="0" t="inlineStr"/>
-      <c r="M55" s="0" t="inlineStr"/>
-      <c r="N55" s="0" t="inlineStr"/>
       <c r="R55" s="0" t="inlineStr">
         <is>
           <t>DS13, pMU770 in strain DS3</t>
@@ -3314,10 +3270,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="K59" s="0" t="inlineStr"/>
-      <c r="L59" s="0" t="inlineStr"/>
-      <c r="M59" s="0" t="inlineStr"/>
-      <c r="N59" s="0" t="inlineStr"/>
       <c r="R59" s="0" t="inlineStr">
         <is>
           <t>DS17, R-M deletion using plasmid pDGO-48</t>
@@ -3369,10 +3321,6 @@
           <t>LL1018</t>
         </is>
       </c>
-      <c r="K60" s="0" t="inlineStr"/>
-      <c r="L60" s="0" t="inlineStr"/>
-      <c r="M60" s="0" t="inlineStr"/>
-      <c r="N60" s="0" t="inlineStr"/>
       <c r="R60" s="0" t="inlineStr">
         <is>
           <t>DS18, DO114.11, plasmid pDGO-37 (empty vector used for cipA complementation) in strain DS16</t>
@@ -3425,10 +3373,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="K61" s="0" t="inlineStr"/>
-      <c r="L61" s="0" t="inlineStr"/>
-      <c r="M61" s="0" t="inlineStr"/>
-      <c r="N61" s="0" t="inlineStr"/>
       <c r="R61" s="0" t="inlineStr">
         <is>
           <t>DS19, DO116.3.4, plasmid pDGO-37 (empty vector used for cipA complementation) in strain DS3</t>
@@ -3649,13 +3593,11 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H65" s="0" t="inlineStr"/>
       <c r="R65" s="0" t="inlineStr">
         <is>
           <t>DS23, T sacch, wild type T. saccharolyticum JW/SL-YS485 from Joe Shaw</t>
         </is>
       </c>
-      <c r="T65" s="0" t="inlineStr"/>
       <c r="U65" s="0" t="b">
         <v>0</v>
       </c>
@@ -3715,13 +3657,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P66" s="0" t="inlineStr"/>
       <c r="R66" s="0" t="inlineStr">
         <is>
           <t>YD01</t>
         </is>
       </c>
-      <c r="S66" s="0" t="inlineStr"/>
       <c r="T66" s="0" t="inlineStr">
         <is>
           <t>LL1010  ∆hpt ∆ldh::Peno-pyk(Tsc)_x000d_
@@ -3841,7 +3781,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="I68" s="0" t="inlineStr"/>
       <c r="K68" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -3862,13 +3801,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P68" s="0" t="inlineStr"/>
       <c r="R68" s="0" t="inlineStr">
         <is>
           <t>∆cipA XDocII.  This strain was given to Julie Paye on 11/6/2012</t>
         </is>
       </c>
-      <c r="S68" s="0" t="inlineStr"/>
       <c r="T68" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -3897,7 +3834,6 @@
       <c r="C69" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D69" s="0" t="inlineStr"/>
       <c r="E69" s="0" t="b">
         <v>0</v>
       </c>
@@ -3936,14 +3872,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P69" s="0" t="inlineStr"/>
-      <c r="Q69" s="0" t="inlineStr"/>
       <c r="R69" s="0" t="inlineStr">
         <is>
           <t>∆cipA XDocII</t>
         </is>
       </c>
-      <c r="S69" s="0" t="inlineStr"/>
       <c r="T69" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -3990,8 +3923,6 @@
           <t>LL1026</t>
         </is>
       </c>
-      <c r="K70" s="0" t="inlineStr"/>
-      <c r="P70" s="0" t="inlineStr"/>
       <c r="R70" s="0" t="inlineStr">
         <is>
           <t>YD05</t>
@@ -4027,7 +3958,6 @@
       <c r="C71" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="D71" s="0" t="inlineStr"/>
       <c r="E71" s="0" t="b">
         <v>0</v>
       </c>
@@ -4046,17 +3976,11 @@
           <t>LL1030</t>
         </is>
       </c>
-      <c r="K71" s="0" t="inlineStr"/>
-      <c r="L71" s="0" t="inlineStr"/>
-      <c r="M71" s="0" t="inlineStr"/>
-      <c r="N71" s="0" t="inlineStr"/>
-      <c r="P71" s="0" t="inlineStr"/>
       <c r="R71" s="0" t="inlineStr">
         <is>
           <t>YD08 (contains plasmid pYD10)</t>
         </is>
       </c>
-      <c r="S71" s="0" t="inlineStr"/>
       <c r="T71" s="0" t="inlineStr">
         <is>
           <t>LL1030 _x000d_
@@ -4106,17 +4030,11 @@
           <t>LL1026</t>
         </is>
       </c>
-      <c r="K72" s="0" t="inlineStr"/>
-      <c r="L72" s="0" t="inlineStr"/>
-      <c r="M72" s="0" t="inlineStr"/>
-      <c r="N72" s="0" t="inlineStr"/>
-      <c r="P72" s="0" t="inlineStr"/>
       <c r="R72" s="0" t="inlineStr">
         <is>
           <t>YD12 (contains plasmid pYD10)</t>
         </is>
       </c>
-      <c r="S72" s="0" t="inlineStr"/>
       <c r="T72" s="0" t="inlineStr">
         <is>
           <t>LL1026 _x000d_
@@ -4190,7 +4108,6 @@
       <c r="U73" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V73" s="0" t="inlineStr"/>
       <c r="Y73" s="0" t="inlineStr">
         <is>
           <t>1033</t>
@@ -4209,7 +4126,6 @@
       <c r="C74" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D74" s="0" t="inlineStr"/>
       <c r="E74" s="0" t="b">
         <v>0</v>
       </c>
@@ -4228,14 +4144,11 @@
           <t>LL1004</t>
         </is>
       </c>
-      <c r="P74" s="0" t="inlineStr"/>
-      <c r="Q74" s="0" t="inlineStr"/>
       <c r="R74" s="0" t="inlineStr">
         <is>
           <t>Tian's attempt to transform plasmid pYD10 into wt C. therm</t>
         </is>
       </c>
-      <c r="S74" s="0" t="inlineStr"/>
       <c r="T74" s="0" t="inlineStr">
         <is>
           <t>LL1004 _x000d_
@@ -4263,7 +4176,6 @@
       <c r="C75" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D75" s="0" t="inlineStr"/>
       <c r="E75" s="0" t="b">
         <v>1</v>
       </c>
@@ -4312,7 +4224,6 @@
           <t>Marybeth Maloney notebook #9 p.4, gel lane 1 (next to 1kb ladder)</t>
         </is>
       </c>
-      <c r="Q75" s="0" t="inlineStr"/>
       <c r="R75" s="0" t="inlineStr">
         <is>
           <t>2nd failed R-M deletion using plasmid pDGO-63.  Plasmid appears to be integrated on genome.</t>
@@ -4442,7 +4353,6 @@
       <c r="C77" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D77" s="0" t="inlineStr"/>
       <c r="E77" s="0" t="b">
         <v>0</v>
       </c>
@@ -4471,13 +4381,11 @@
           <t>Yu Deng gave this strain to Marybeth and she put it directly in the culture collection (i.e. did not subculture)</t>
         </is>
       </c>
-      <c r="Q77" s="0" t="inlineStr"/>
       <c r="R77" s="0" t="inlineStr">
         <is>
           <t>New YD02.  Original YD02 seemed to be contaminated when we did genome sequencing.  See Dan Olson lab notebook #11, p. 69 for details.</t>
         </is>
       </c>
-      <c r="S77" s="0" t="inlineStr"/>
       <c r="T77" s="0" t="inlineStr">
         <is>
           <t>LL1010  ∆hpt ∆ldh::Peno-pyk(Tsc)_x000d_
@@ -4555,7 +4463,6 @@
           <t>Dan Olson, notebook 11, p. 86=7 (copy of confirmation PCR done by Adam Guss).  See additional confirmation in Dan Olson's lab notebook 12 p. 24</t>
         </is>
       </c>
-      <c r="Q78" s="0" t="inlineStr"/>
       <c r="R78" s="0" t="inlineStr">
         <is>
           <t>ldh adhE*, adhE*∆ldh 2-F2C3 from Adam Guss</t>
@@ -4638,7 +4545,6 @@
           <t>Dan Olson, notebook 11, p. 86=7 (copy of confirmation PCR done by Adam Guss)</t>
         </is>
       </c>
-      <c r="Q79" s="0" t="inlineStr"/>
       <c r="R79" s="0" t="inlineStr">
         <is>
           <t>2QKO 2-1, quad knockout, from Adam Guss Same as strain LL1199.  LL1199 is the official "quad mutant" strain.  Parent strain may not be correct.</t>
@@ -4698,7 +4604,6 @@
           <t>LL1179</t>
         </is>
       </c>
-      <c r="Q80" s="0" t="inlineStr"/>
       <c r="R80" s="0" t="inlineStr">
         <is>
           <t>DS24, ALK2.  We weren't able to revive LL439, so we started another culture from Dan Olson's DS24 stock.  Ethanologen.</t>
@@ -4907,11 +4812,6 @@
           <t>LL1042</t>
         </is>
       </c>
-      <c r="I83" s="0" t="inlineStr"/>
-      <c r="K83" s="0" t="inlineStr"/>
-      <c r="L83" s="0" t="inlineStr"/>
-      <c r="M83" s="0" t="inlineStr"/>
-      <c r="N83" s="0" t="inlineStr"/>
       <c r="P83" s="0" t="inlineStr">
         <is>
           <t>See Dan Olson notebook 12 p. 24 for details of PCR confirmation</t>
@@ -4985,11 +4885,6 @@
           <t>LL372</t>
         </is>
       </c>
-      <c r="I84" s="0" t="inlineStr"/>
-      <c r="K84" s="0" t="inlineStr"/>
-      <c r="L84" s="0" t="inlineStr"/>
-      <c r="M84" s="0" t="inlineStr"/>
-      <c r="N84" s="0" t="inlineStr"/>
       <c r="P84" s="0" t="inlineStr">
         <is>
           <t>See Dan Olson notebook 12 p. 24 for details of PCR confirmation.  Note that this strain appears to be merodiploid at the pta locus.</t>
@@ -5053,13 +4948,6 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="H85" s="0" t="inlineStr"/>
-      <c r="I85" s="0" t="inlineStr"/>
-      <c r="K85" s="0" t="inlineStr"/>
-      <c r="L85" s="0" t="inlineStr"/>
-      <c r="M85" s="0" t="inlineStr"/>
-      <c r="N85" s="0" t="inlineStr"/>
-      <c r="P85" s="0" t="inlineStr"/>
       <c r="Q85" s="0" t="inlineStr">
         <is>
           <t>M1074</t>
@@ -5075,7 +4963,6 @@
           <t> ∆pyrF ∆rnf</t>
         </is>
       </c>
-      <c r="T85" s="0" t="inlineStr"/>
       <c r="U85" s="0" t="b">
         <v>0</v>
       </c>
@@ -5110,7 +4997,6 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="K86" s="0" t="inlineStr"/>
       <c r="Q86" s="0" t="inlineStr">
         <is>
           <t>M1075</t>
@@ -5160,7 +5046,6 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="K87" s="0" t="inlineStr"/>
       <c r="Q87" s="0" t="inlineStr">
         <is>
           <t>M1571</t>
@@ -5215,7 +5100,6 @@
           <t>LL1004</t>
         </is>
       </c>
-      <c r="K88" s="0" t="inlineStr"/>
       <c r="Q88" s="0" t="inlineStr">
         <is>
           <t>M1572</t>
@@ -5271,8 +5155,6 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H89" s="0" t="inlineStr"/>
-      <c r="K89" s="0" t="inlineStr"/>
       <c r="Q89" s="0" t="inlineStr">
         <is>
           <t>M1442</t>
@@ -5288,7 +5170,6 @@
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure Δeps</t>
         </is>
       </c>
-      <c r="T89" s="0" t="inlineStr"/>
       <c r="U89" s="0" t="b">
         <v>0</v>
       </c>
@@ -5567,24 +5448,19 @@
           <t>Thermoanaerobacterium thermosaccharolyticum DSM 571</t>
         </is>
       </c>
-      <c r="H93" s="0" t="inlineStr"/>
       <c r="K93" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="P93" s="0" t="inlineStr"/>
       <c r="R93" s="0" t="inlineStr">
         <is>
           <t>Wild type strain from DSMZ</t>
         </is>
       </c>
-      <c r="S93" s="0" t="inlineStr"/>
-      <c r="T93" s="0" t="inlineStr"/>
       <c r="U93" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V93" s="0" t="inlineStr"/>
       <c r="Y93" s="0" t="inlineStr">
         <is>
           <t>1053</t>
@@ -5616,7 +5492,6 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H94" s="0" t="inlineStr"/>
       <c r="K94" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -5627,7 +5502,6 @@
           <t>Wild type (not sure where it came from originally)</t>
         </is>
       </c>
-      <c r="T94" s="0" t="inlineStr"/>
       <c r="U94" s="0" t="b">
         <v>0</v>
       </c>
@@ -5901,16 +5775,11 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L99" s="0" t="inlineStr"/>
-      <c r="M99" s="0" t="inlineStr"/>
-      <c r="N99" s="0" t="inlineStr"/>
-      <c r="P99" s="0" t="inlineStr"/>
       <c r="R99" s="0" t="inlineStr">
         <is>
           <t>bcd eftA etfB genes from T. thermosaccharolyticum DSM 571 inserted into T. saccharolyticum</t>
         </is>
       </c>
-      <c r="S99" s="0" t="inlineStr"/>
       <c r="T99" s="0" t="inlineStr">
         <is>
           <t>LL440  ∆pyrF ∆(pta-ack) ∆ldh Δxyl_x000d_
@@ -5943,7 +5812,6 @@
       <c r="C100" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D100" s="0" t="inlineStr"/>
       <c r="E100" s="0" t="b">
         <v>0</v>
       </c>
@@ -5967,9 +5835,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L100" s="0" t="inlineStr"/>
-      <c r="M100" s="0" t="inlineStr"/>
-      <c r="N100" s="0" t="inlineStr"/>
       <c r="P100" s="0" t="inlineStr">
         <is>
           <t>Ashie Bhandiwad notebook #3, p. 5</t>
@@ -6021,7 +5886,6 @@
       <c r="C101" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D101" s="0" t="inlineStr"/>
       <c r="E101" s="0" t="b">
         <v>0</v>
       </c>
@@ -6045,16 +5909,11 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L101" s="0" t="inlineStr"/>
-      <c r="M101" s="0" t="inlineStr"/>
-      <c r="N101" s="0" t="inlineStr"/>
-      <c r="P101" s="0" t="inlineStr"/>
       <c r="R101" s="0" t="inlineStr">
         <is>
           <t>thl hbd crt bcd etfAB and adhE deletion</t>
         </is>
       </c>
-      <c r="S101" s="0" t="inlineStr"/>
       <c r="T101" s="0" t="inlineStr">
         <is>
           <t>LL1025 _x000d_
@@ -6082,7 +5941,6 @@
       <c r="C102" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D102" s="0" t="inlineStr"/>
       <c r="E102" s="0" t="b">
         <v>0</v>
       </c>
@@ -6096,23 +5954,16 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H102" s="0" t="inlineStr"/>
       <c r="K102" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L102" s="0" t="inlineStr"/>
-      <c r="M102" s="0" t="inlineStr"/>
-      <c r="N102" s="0" t="inlineStr"/>
-      <c r="P102" s="0" t="inlineStr"/>
       <c r="R102" s="0" t="inlineStr">
         <is>
           <t>thl hbd crt bcd etfAB and adhE deletion in strain MO210 from Mascoma</t>
         </is>
       </c>
-      <c r="S102" s="0" t="inlineStr"/>
-      <c r="T102" s="0" t="inlineStr"/>
       <c r="U102" s="0" t="b">
         <v>0</v>
       </c>
@@ -6134,7 +5985,6 @@
       <c r="C103" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D103" s="0" t="inlineStr"/>
       <c r="E103" s="0" t="b">
         <v>0</v>
       </c>
@@ -6148,23 +5998,16 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H103" s="0" t="inlineStr"/>
       <c r="K103" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L103" s="0" t="inlineStr"/>
-      <c r="M103" s="0" t="inlineStr"/>
-      <c r="N103" s="0" t="inlineStr"/>
-      <c r="P103" s="0" t="inlineStr"/>
       <c r="R103" s="0" t="inlineStr">
         <is>
           <t>thl hbd crt bcd etfAB and adhE deletion in strain MO210 from Mascoma (same as previous strain, as far as Dan Olson knows)</t>
         </is>
       </c>
-      <c r="S103" s="0" t="inlineStr"/>
-      <c r="T103" s="0" t="inlineStr"/>
       <c r="U103" s="0" t="b">
         <v>0</v>
       </c>
@@ -6186,7 +6029,6 @@
       <c r="C104" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D104" s="0" t="inlineStr"/>
       <c r="E104" s="0" t="b">
         <v>0</v>
       </c>
@@ -6210,16 +6052,11 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L104" s="0" t="inlineStr"/>
-      <c r="M104" s="0" t="inlineStr"/>
-      <c r="N104" s="0" t="inlineStr"/>
-      <c r="P104" s="0" t="inlineStr"/>
       <c r="R104" s="0" t="inlineStr">
         <is>
           <t>ldh deletion in T. thermosacch</t>
         </is>
       </c>
-      <c r="S104" s="0" t="inlineStr"/>
       <c r="T104" s="0" t="inlineStr">
         <is>
           <t>LL1053 _x000d_
@@ -6270,13 +6107,11 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="Q105" s="0" t="inlineStr"/>
       <c r="R105" s="0" t="inlineStr">
         <is>
           <t>adhE deletion in T. thermosacch</t>
         </is>
       </c>
-      <c r="S105" s="0" t="inlineStr"/>
       <c r="T105" s="0" t="inlineStr">
         <is>
           <t>LL1053 _x000d_
@@ -6347,7 +6182,6 @@
           <t>Dan Olson, notebook 11, p.99, PCR confirmation in notebook 12, p. 25. adhE* mutation was confirmed, but pfl mutation hasn't been confirmed yet.</t>
         </is>
       </c>
-      <c r="Q106" s="0" t="inlineStr"/>
       <c r="R106" s="0" t="inlineStr">
         <is>
           <t>AG01, ∆hpt adhE* ∆pfl</t>
@@ -6435,7 +6269,6 @@
           <t>Dan Olson, notebook 11, p.99, PCR confirmation in notebook 12, p. 25</t>
         </is>
       </c>
-      <c r="Q107" s="0" t="inlineStr"/>
       <c r="R107" s="0" t="inlineStr">
         <is>
           <t>AG02, ∆hpt adhE* ∆ldh, might be the same as LL1038</t>
@@ -6523,7 +6356,6 @@
           <t>Dan Olson, notebook 11, p.99, PCR confirmation in notebook 12, p. 25</t>
         </is>
       </c>
-      <c r="Q108" s="0" t="inlineStr"/>
       <c r="R108" s="0" t="inlineStr">
         <is>
           <t>Labeled as AG03.  Suppose d to have ∆hpt ∆hydG genotype.  Also has pfl deletion (see DO notebook 12 p. 53)._x000d_
@@ -6613,7 +6445,6 @@
           <t>Dan Olson, notebook 11, p.99, PCR confirmation in notebook 12, p. 25</t>
         </is>
       </c>
-      <c r="Q109" s="0" t="inlineStr"/>
       <c r="R109" s="0" t="inlineStr">
         <is>
           <t>RB01, ∆hpt ∆hydG ∆pfl</t>
@@ -6636,7 +6467,6 @@
       <c r="U109" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V109" s="0" t="inlineStr"/>
       <c r="Y109" s="0" t="inlineStr">
         <is>
           <t>1069</t>
@@ -6703,7 +6533,6 @@
           <t>Dan Olson, notebook 11, p.99, PCR confirmation in notebook 12, p. 25</t>
         </is>
       </c>
-      <c r="Q110" s="0" t="inlineStr"/>
       <c r="R110" s="0" t="inlineStr">
         <is>
           <t>Strain from Adam Guss lab, send by Ranjita, labeled as RB02.  Genotype is supposed to be ∆hpt ∆hydG ∆ldh.  Based on PCR, I though we had found and additional pfl deletion (DO notebook 12 p. 53).  Based on resequencing data from JGI, the pfl locus is wild type.  Sequencing data shows presence of bacteriophage S13.</t>
@@ -6767,7 +6596,6 @@
           <t>LL1068</t>
         </is>
       </c>
-      <c r="I111" s="0" t="inlineStr"/>
       <c r="K111" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -6858,10 +6686,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L112" s="0" t="inlineStr"/>
-      <c r="M112" s="0" t="inlineStr"/>
-      <c r="N112" s="0" t="inlineStr"/>
-      <c r="P112" s="0" t="inlineStr"/>
       <c r="Q112" s="0" t="inlineStr">
         <is>
           <t>M5300</t>
@@ -6927,10 +6751,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L113" s="0" t="inlineStr"/>
-      <c r="M113" s="0" t="inlineStr"/>
-      <c r="N113" s="0" t="inlineStr"/>
-      <c r="P113" s="0" t="inlineStr"/>
       <c r="Q113" s="0" t="inlineStr">
         <is>
           <t>M5676</t>
@@ -6994,10 +6814,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L114" s="0" t="inlineStr"/>
-      <c r="M114" s="0" t="inlineStr"/>
-      <c r="N114" s="0" t="inlineStr"/>
-      <c r="P114" s="0" t="inlineStr"/>
       <c r="Q114" s="0" t="inlineStr">
         <is>
           <t>M5678</t>
@@ -7061,10 +6877,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L115" s="0" t="inlineStr"/>
-      <c r="M115" s="0" t="inlineStr"/>
-      <c r="N115" s="0" t="inlineStr"/>
-      <c r="P115" s="0" t="inlineStr"/>
       <c r="Q115" s="0" t="inlineStr">
         <is>
           <t>M5680</t>
@@ -7123,7 +6935,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="I116" s="0" t="inlineStr"/>
       <c r="K116" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -7144,7 +6955,6 @@
           <t>xylose</t>
         </is>
       </c>
-      <c r="P116" s="0" t="inlineStr"/>
       <c r="Q116" s="0" t="inlineStr">
         <is>
           <t>M3223</t>
@@ -7174,8 +6984,6 @@
           <t>DO notebook 16 p.38</t>
         </is>
       </c>
-      <c r="W116" s="0" t="inlineStr"/>
-      <c r="X116" s="0" t="inlineStr"/>
       <c r="Y116" s="0" t="inlineStr">
         <is>
           <t>1076</t>
@@ -7207,8 +7015,6 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H117" s="0" t="inlineStr"/>
-      <c r="I117" s="0" t="inlineStr"/>
       <c r="K117" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -7229,7 +7035,6 @@
           <t>xylose</t>
         </is>
       </c>
-      <c r="P117" s="0" t="inlineStr"/>
       <c r="Q117" s="0" t="inlineStr">
         <is>
           <t>M3224</t>
@@ -7240,13 +7045,9 @@
           <t>M3224, M0355 + adhE deletion, with pta ack kanR, furfural stimulates growth</t>
         </is>
       </c>
-      <c r="S117" s="0" t="inlineStr"/>
-      <c r="T117" s="0" t="inlineStr"/>
       <c r="U117" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W117" s="0" t="inlineStr"/>
-      <c r="X117" s="0" t="inlineStr"/>
       <c r="Y117" s="0" t="inlineStr">
         <is>
           <t>1077</t>
@@ -7308,9 +7109,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P118" s="0" t="inlineStr"/>
-      <c r="R118" s="0" t="inlineStr"/>
-      <c r="S118" s="0" t="inlineStr"/>
       <c r="T118" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -7322,8 +7120,6 @@
       <c r="U118" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W118" s="0" t="inlineStr"/>
-      <c r="X118" s="0" t="inlineStr"/>
       <c r="Y118" s="0" t="inlineStr">
         <is>
           <t>1078</t>
@@ -7360,7 +7156,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="I119" s="0" t="inlineStr"/>
       <c r="K119" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -7391,7 +7186,6 @@
           <t>Cthe_0256 KO, histidine kinase related to sporulation</t>
         </is>
       </c>
-      <c r="S119" s="0" t="inlineStr"/>
       <c r="T119" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -7402,8 +7196,6 @@
       <c r="U119" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W119" s="0" t="inlineStr"/>
-      <c r="X119" s="0" t="inlineStr"/>
       <c r="Y119" s="0" t="inlineStr">
         <is>
           <t>1079</t>
@@ -7440,7 +7232,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="I120" s="0" t="inlineStr"/>
       <c r="K120" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -7471,7 +7262,6 @@
           <t>Cthe_2076 KO, histidine kinase related to sporulation</t>
         </is>
       </c>
-      <c r="S120" s="0" t="inlineStr"/>
       <c r="T120" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -7482,8 +7272,6 @@
       <c r="U120" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W120" s="0" t="inlineStr"/>
-      <c r="X120" s="0" t="inlineStr"/>
       <c r="Y120" s="0" t="inlineStr">
         <is>
           <t>1080</t>
@@ -7520,7 +7308,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="I121" s="0" t="inlineStr"/>
       <c r="K121" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -7597,7 +7384,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="I122" s="0" t="inlineStr"/>
       <c r="K122" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -9049,11 +8835,6 @@
           <t>pMU3603</t>
         </is>
       </c>
-      <c r="K139" s="0" t="inlineStr"/>
-      <c r="L139" s="0" t="inlineStr"/>
-      <c r="M139" s="0" t="inlineStr"/>
-      <c r="N139" s="0" t="inlineStr"/>
-      <c r="P139" s="0" t="inlineStr"/>
       <c r="R139" s="0" t="inlineStr">
         <is>
           <t>C. thermocellum FAE triple KO genes 1305+2635+2858 colony 1, 1313_1305+2635+2858 markerless FAE domain KO, derived from LL1074 by using pMU3603</t>
@@ -9111,13 +8892,11 @@
           <t>pMU3603</t>
         </is>
       </c>
-      <c r="P140" s="0" t="inlineStr"/>
       <c r="R140" s="0" t="inlineStr">
         <is>
           <t>C. thermocellum FAE triple KO genes 1305+2635+2858 colony 4, 1313_1305+2635+2858 markerless FAE domain KO, derived from LL1074 by using pMU3603</t>
         </is>
       </c>
-      <c r="S140" s="0" t="inlineStr"/>
       <c r="T140" s="0" t="inlineStr">
         <is>
           <t>LL1074 _x000d_
@@ -9195,7 +8974,6 @@
           <t>Δ0286Δ0256</t>
         </is>
       </c>
-      <c r="S141" s="0" t="inlineStr"/>
       <c r="T141" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -9272,7 +9050,6 @@
           <t>Δ0286Δ2076</t>
         </is>
       </c>
-      <c r="S142" s="0" t="inlineStr"/>
       <c r="T142" s="0" t="inlineStr">
         <is>
           <t>LL346  adhE*_x000d_
@@ -9349,7 +9126,6 @@
           <t>Δ0286Δ2677</t>
         </is>
       </c>
-      <c r="S143" s="0" t="inlineStr"/>
       <c r="T143" s="0" t="inlineStr">
         <is>
           <t>LL347 _x000d_
@@ -9395,7 +9171,6 @@
           <t>LL348</t>
         </is>
       </c>
-      <c r="I144" s="0" t="inlineStr"/>
       <c r="K144" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -9426,7 +9201,6 @@
           <t>Δ2677Δ0256</t>
         </is>
       </c>
-      <c r="S144" s="0" t="inlineStr"/>
       <c r="T144" s="0" t="inlineStr">
         <is>
           <t>LL348 _x000d_
@@ -9502,7 +9276,6 @@
           <t>Δ2677Δ2076</t>
         </is>
       </c>
-      <c r="S145" s="0" t="inlineStr"/>
       <c r="T145" s="0" t="inlineStr">
         <is>
           <t>LL349  ∆hpt ∆ech_x000d_
@@ -9580,7 +9353,6 @@
           <t>Δ2076Δ0256</t>
         </is>
       </c>
-      <c r="S146" s="0" t="inlineStr"/>
       <c r="T146" s="0" t="inlineStr">
         <is>
           <t>LL350  adhE D494G ∆hpt ∆hydG_x000d_
@@ -9628,7 +9400,6 @@
           <t>LL1011</t>
         </is>
       </c>
-      <c r="I147" s="0" t="inlineStr"/>
       <c r="P147" s="0" t="inlineStr">
         <is>
           <t>MB notebook 10, p. 29</t>
@@ -9657,8 +9428,6 @@
       <c r="U147" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W147" s="0" t="inlineStr"/>
-      <c r="X147" s="0" t="inlineStr"/>
       <c r="Y147" s="0" t="inlineStr">
         <is>
           <t>1107</t>
@@ -9695,9 +9464,6 @@
           <t>LL1044</t>
         </is>
       </c>
-      <c r="L148" s="0" t="inlineStr"/>
-      <c r="M148" s="0" t="inlineStr"/>
-      <c r="N148" s="0" t="inlineStr"/>
       <c r="P148" s="0" t="inlineStr">
         <is>
           <t>MB notebook 10, p. 29</t>
@@ -9762,11 +9528,6 @@
           <t>LL1043</t>
         </is>
       </c>
-      <c r="I149" s="0" t="inlineStr"/>
-      <c r="K149" s="0" t="inlineStr"/>
-      <c r="L149" s="0" t="inlineStr"/>
-      <c r="M149" s="0" t="inlineStr"/>
-      <c r="N149" s="0" t="inlineStr"/>
       <c r="P149" s="0" t="inlineStr">
         <is>
           <t>MB notebook 10, p. 29</t>
@@ -9831,12 +9592,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="I150" s="0" t="inlineStr"/>
-      <c r="K150" s="0" t="inlineStr"/>
-      <c r="L150" s="0" t="inlineStr"/>
-      <c r="M150" s="0" t="inlineStr"/>
-      <c r="N150" s="0" t="inlineStr"/>
-      <c r="P150" s="0" t="inlineStr"/>
       <c r="R150" s="0" t="inlineStr">
         <is>
           <t>peps deletion</t>
@@ -9898,10 +9653,6 @@
           <t>pJLO19</t>
         </is>
       </c>
-      <c r="K151" s="0" t="inlineStr"/>
-      <c r="L151" s="0" t="inlineStr"/>
-      <c r="M151" s="0" t="inlineStr"/>
-      <c r="N151" s="0" t="inlineStr"/>
       <c r="P151" s="0" t="inlineStr">
         <is>
           <t>1/20/2015 Marybeth had a freezer stock that was contaminated, but the master stocks were fine.  Marybeth made new freezer stocks from the master.  These stocks were confirmed to be correct by Shuen.  See SH Book V, p. 68 for details.</t>
@@ -9963,12 +9714,6 @@
           <t>LL1010</t>
         </is>
       </c>
-      <c r="I152" s="0" t="inlineStr"/>
-      <c r="K152" s="0" t="inlineStr"/>
-      <c r="L152" s="0" t="inlineStr"/>
-      <c r="M152" s="0" t="inlineStr"/>
-      <c r="N152" s="0" t="inlineStr"/>
-      <c r="P152" s="0" t="inlineStr"/>
       <c r="R152" s="0" t="inlineStr">
         <is>
           <t>new YD01 strain.  Was supposed to have ATG --&gt; GTG start codon change at PEPCK, but that was not observed by Sanger sequencing.  Does not appear to be any different from LL1010.</t>
@@ -10026,12 +9771,6 @@
           <t>LL1010</t>
         </is>
       </c>
-      <c r="I153" s="0" t="inlineStr"/>
-      <c r="K153" s="0" t="inlineStr"/>
-      <c r="L153" s="0" t="inlineStr"/>
-      <c r="M153" s="0" t="inlineStr"/>
-      <c r="N153" s="0" t="inlineStr"/>
-      <c r="P153" s="0" t="inlineStr"/>
       <c r="R153" s="0" t="inlineStr">
         <is>
           <t>new YD02 strain, reconstructed from LL1010 with plasmid pYD14</t>
@@ -10094,10 +9833,6 @@
           <t>pJLO13 and pJLo17</t>
         </is>
       </c>
-      <c r="K154" s="0" t="inlineStr"/>
-      <c r="L154" s="0" t="inlineStr"/>
-      <c r="M154" s="0" t="inlineStr"/>
-      <c r="N154" s="0" t="inlineStr"/>
       <c r="P154" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 5, page 27-29</t>
@@ -10156,15 +9891,11 @@
       <c r="E155" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="F155" s="0" t="inlineStr"/>
       <c r="G155" s="0" t="inlineStr">
         <is>
           <t>Thermoanaerobacter ethanolicus ATCC 31550</t>
         </is>
       </c>
-      <c r="H155" s="0" t="inlineStr"/>
-      <c r="I155" s="0" t="inlineStr"/>
-      <c r="K155" s="0" t="inlineStr"/>
       <c r="L155" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -10180,13 +9911,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P155" s="0" t="inlineStr"/>
       <c r="R155" s="0" t="inlineStr">
         <is>
           <t>Tian got it from from ATCC in order to clone the adhE.  It's strain JW200.</t>
         </is>
       </c>
-      <c r="T155" s="0" t="inlineStr"/>
       <c r="U155" s="0" t="b">
         <v>0</v>
       </c>
@@ -11401,7 +11130,6 @@
           <t>1726:118</t>
         </is>
       </c>
-      <c r="S170" s="0" t="inlineStr"/>
       <c r="T170" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -11479,13 +11207,11 @@
           <t>NB 7, page 65</t>
         </is>
       </c>
-      <c r="Q171" s="0" t="inlineStr"/>
       <c r="R171" s="0" t="inlineStr">
         <is>
           <t>1726:119</t>
         </is>
       </c>
-      <c r="S171" s="0" t="inlineStr"/>
       <c r="T171" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -11568,7 +11294,6 @@
           <t>1726:120</t>
         </is>
       </c>
-      <c r="S172" s="0" t="inlineStr"/>
       <c r="T172" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -11651,7 +11376,6 @@
           <t>1726:121</t>
         </is>
       </c>
-      <c r="S173" s="0" t="inlineStr"/>
       <c r="T173" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -11734,7 +11458,6 @@
           <t>1726:122</t>
         </is>
       </c>
-      <c r="S174" s="0" t="inlineStr"/>
       <c r="T174" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -11817,7 +11540,6 @@
           <t>1726:123</t>
         </is>
       </c>
-      <c r="S175" s="0" t="inlineStr"/>
       <c r="T175" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -11895,13 +11617,11 @@
           <t>NB 7, page 65</t>
         </is>
       </c>
-      <c r="Q176" s="0" t="inlineStr"/>
       <c r="R176" s="0" t="inlineStr">
         <is>
           <t>1726:205</t>
         </is>
       </c>
-      <c r="S176" s="0" t="inlineStr"/>
       <c r="T176" s="0" t="inlineStr">
         <is>
           <t>LL376  ∆hpt ∆spo0A_x000d_
@@ -11949,7 +11669,6 @@
           <t>LL1113</t>
         </is>
       </c>
-      <c r="I177" s="0" t="inlineStr"/>
       <c r="L177" s="0" t="inlineStr">
         <is>
           <t>MTC</t>
@@ -12028,7 +11747,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="I178" s="0" t="inlineStr"/>
       <c r="L178" s="0" t="inlineStr">
         <is>
           <t>MTC</t>
@@ -12120,7 +11838,6 @@
           <t>Jilai Zhou, Notebook 4, p. 99 (PCR confirmation of deletion region)</t>
         </is>
       </c>
-      <c r="Q179" s="0" t="inlineStr"/>
       <c r="R179" s="0" t="inlineStr">
         <is>
           <t>Δpfor::kan, colony-9</t>
@@ -12181,9 +11898,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L180" s="0" t="inlineStr"/>
-      <c r="M180" s="0" t="inlineStr"/>
-      <c r="N180" s="0" t="inlineStr"/>
       <c r="P180" s="0" t="inlineStr">
         <is>
           <t>Jilai Zhou, Notebook 4, p. 99 (PCR confirmation of deletion region)</t>
@@ -12249,9 +11963,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L181" s="0" t="inlineStr"/>
-      <c r="M181" s="0" t="inlineStr"/>
-      <c r="N181" s="0" t="inlineStr"/>
       <c r="P181" s="0" t="inlineStr">
         <is>
           <t>Jilai Zhou, Notebook 5, p. 26</t>
@@ -12318,9 +12029,6 @@
           <t>20% glycerol, 30% water, 50% culture</t>
         </is>
       </c>
-      <c r="L182" s="0" t="inlineStr"/>
-      <c r="M182" s="0" t="inlineStr"/>
-      <c r="N182" s="0" t="inlineStr"/>
       <c r="P182" s="0" t="inlineStr">
         <is>
           <t>Jilai Zhou, Notebook 5, p. 26</t>
@@ -12382,9 +12090,6 @@
           <t>LL1185</t>
         </is>
       </c>
-      <c r="L183" s="0" t="inlineStr"/>
-      <c r="M183" s="0" t="inlineStr"/>
-      <c r="N183" s="0" t="inlineStr"/>
       <c r="P183" s="0" t="inlineStr">
         <is>
           <t>Strain received from Mascoma, through tech transfer</t>
@@ -12457,9 +12162,6 @@
           <t>pMU804</t>
         </is>
       </c>
-      <c r="L184" s="0" t="inlineStr"/>
-      <c r="M184" s="0" t="inlineStr"/>
-      <c r="N184" s="0" t="inlineStr"/>
       <c r="P184" s="0" t="inlineStr">
         <is>
           <t>Strain received from Mascoma, through tech transfer, made by Shital</t>
@@ -12525,10 +12227,6 @@
           <t>Used PCR from ST86</t>
         </is>
       </c>
-      <c r="K185" s="0" t="inlineStr"/>
-      <c r="L185" s="0" t="inlineStr"/>
-      <c r="M185" s="0" t="inlineStr"/>
-      <c r="N185" s="0" t="inlineStr"/>
       <c r="P185" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 5, page 40-41</t>
@@ -12556,8 +12254,6 @@
       <c r="U185" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W185" s="0" t="inlineStr"/>
-      <c r="X185" s="0" t="inlineStr"/>
       <c r="Y185" s="0" t="inlineStr">
         <is>
           <t>1145</t>
@@ -12594,7 +12290,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="I186" s="0" t="inlineStr"/>
       <c r="P186" s="0" t="inlineStr">
         <is>
           <t>Strain received from Mascoma, through tech transfer</t>
@@ -12660,7 +12355,6 @@
           <t>LL350</t>
         </is>
       </c>
-      <c r="I187" s="0" t="inlineStr"/>
       <c r="K187" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -12911,7 +12605,6 @@
           <t>Caldicellulosiruptor bescii</t>
         </is>
       </c>
-      <c r="H190" s="0" t="inlineStr"/>
       <c r="L190" s="0" t="inlineStr">
         <is>
           <t>Bescii DSM medium</t>
@@ -12927,9 +12620,6 @@
           <t>0</t>
         </is>
       </c>
-      <c r="R190" s="0" t="inlineStr"/>
-      <c r="S190" s="0" t="inlineStr"/>
-      <c r="T190" s="0" t="inlineStr"/>
       <c r="U190" s="0" t="b">
         <v>0</v>
       </c>
@@ -12964,8 +12654,6 @@
           <t>Caldicellulosiruptor obsidianis</t>
         </is>
       </c>
-      <c r="H191" s="0" t="inlineStr"/>
-      <c r="K191" s="0" t="inlineStr"/>
       <c r="L191" s="0" t="inlineStr">
         <is>
           <t>Bescii DSM medium</t>
@@ -12986,8 +12674,6 @@
           <t>OB47</t>
         </is>
       </c>
-      <c r="S191" s="0" t="inlineStr"/>
-      <c r="T191" s="0" t="inlineStr"/>
       <c r="U191" s="0" t="b">
         <v>0</v>
       </c>
@@ -13248,8 +12934,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="I195" s="0" t="inlineStr"/>
-      <c r="P195" s="0" t="inlineStr"/>
       <c r="R195" s="0" t="inlineStr">
         <is>
           <t>Tsac_1067 deletion</t>
@@ -13324,7 +13008,6 @@
       <c r="U196" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V196" s="0" t="inlineStr"/>
       <c r="Y196" s="0" t="inlineStr">
         <is>
           <t>1156</t>
@@ -13380,7 +13063,6 @@
       <c r="U197" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V197" s="0" t="inlineStr"/>
       <c r="Y197" s="0" t="inlineStr">
         <is>
           <t>1157</t>
@@ -13444,7 +13126,6 @@
       <c r="U198" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V198" s="0" t="inlineStr"/>
       <c r="Y198" s="0" t="inlineStr">
         <is>
           <t>1158</t>
@@ -13500,7 +13181,6 @@
       <c r="U199" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V199" s="0" t="inlineStr"/>
       <c r="Y199" s="0" t="inlineStr">
         <is>
           <t>1159</t>
@@ -13537,11 +13217,6 @@
           <t>LL1111</t>
         </is>
       </c>
-      <c r="K200" s="0" t="inlineStr"/>
-      <c r="L200" s="0" t="inlineStr"/>
-      <c r="M200" s="0" t="inlineStr"/>
-      <c r="N200" s="0" t="inlineStr"/>
-      <c r="P200" s="0" t="inlineStr"/>
       <c r="R200" s="0" t="inlineStr">
         <is>
           <t>Re-constructed adhE locus by re-introducing wild-type adhE</t>
@@ -13563,7 +13238,6 @@
       <c r="U200" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V200" s="0" t="inlineStr"/>
       <c r="Y200" s="0" t="inlineStr">
         <is>
           <t>1160</t>
@@ -13722,7 +13396,6 @@
           <t>LL1137</t>
         </is>
       </c>
-      <c r="R203" s="0" t="inlineStr"/>
       <c r="S203" s="0" t="inlineStr">
         <is>
           <t> ∆hpt ∆ldh::Peno-pyk(Tsc) ∆me-mdh</t>
@@ -13782,7 +13455,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="P204" s="0" t="inlineStr"/>
       <c r="R204" s="0" t="inlineStr">
         <is>
           <t>pfl deletion based on LL1025</t>
@@ -13843,7 +13515,6 @@
           <t>LL1049</t>
         </is>
       </c>
-      <c r="P205" s="0" t="inlineStr"/>
       <c r="R205" s="0" t="inlineStr">
         <is>
           <t>pfl deltion based on LL1049</t>
@@ -13904,7 +13575,6 @@
           <t>LL1163</t>
         </is>
       </c>
-      <c r="Q206" s="0" t="inlineStr"/>
       <c r="R206" s="0" t="inlineStr">
         <is>
           <t>pta deletion in LL1163, colony #1 (sister colony of LL1169, note that 1166 and 1169 have similar fermentation data, so we are focusing on 1166)</t>
@@ -13965,7 +13635,6 @@
           <t>Thermoanaerobacter pseudethanolicus ATCC 33223</t>
         </is>
       </c>
-      <c r="H207" s="0" t="inlineStr"/>
       <c r="K207" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -13996,8 +13665,6 @@
           <t>T. ethanolicus H8, ethanol-adapted strain from Zeikus lab.   Derived from strain T. pseudoethanolicus 39E, ATCC 33223</t>
         </is>
       </c>
-      <c r="S207" s="0" t="inlineStr"/>
-      <c r="T207" s="0" t="inlineStr"/>
       <c r="U207" s="0" t="b">
         <v>1</v>
       </c>
@@ -14042,7 +13709,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="P208" s="0" t="inlineStr"/>
       <c r="R208" s="0" t="inlineStr">
         <is>
           <t>pfl deletion with erm in LL1025</t>
@@ -14062,7 +13728,6 @@
       <c r="U208" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V208" s="0" t="inlineStr"/>
       <c r="Y208" s="0" t="inlineStr">
         <is>
           <t>1168</t>
@@ -14099,7 +13764,6 @@
           <t>LL1163</t>
         </is>
       </c>
-      <c r="P209" s="0" t="inlineStr"/>
       <c r="R209" s="0" t="inlineStr">
         <is>
           <t>pta deletion in LL1163, colony #2 (sister colony of LL1166)</t>
@@ -14124,7 +13788,6 @@
       <c r="U209" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="V209" s="0" t="inlineStr"/>
       <c r="Y209" s="0" t="inlineStr">
         <is>
           <t>1169</t>
@@ -14161,7 +13824,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="P210" s="0" t="inlineStr"/>
       <c r="R210" s="0" t="inlineStr">
         <is>
           <t>pfl deletion in LL1025 colony #3</t>
@@ -14290,22 +13952,16 @@
           <t>LL1143</t>
         </is>
       </c>
-      <c r="K212" s="0" t="inlineStr"/>
-      <c r="L212" s="0" t="inlineStr"/>
-      <c r="M212" s="0" t="inlineStr"/>
-      <c r="N212" s="0" t="inlineStr"/>
       <c r="P212" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 6, page 21</t>
         </is>
       </c>
-      <c r="Q212" s="0" t="inlineStr"/>
       <c r="R212" s="0" t="inlineStr">
         <is>
           <t>M0353, low ethanol producing colony. Jon Lo could not find this strain and it is presumed lost.</t>
         </is>
       </c>
-      <c r="S212" s="0" t="inlineStr"/>
       <c r="T212" s="0" t="inlineStr">
         <is>
           <t>LL1143  ∆pyrF ∆(pta-ack) ∆ldh_x000d_
@@ -14354,9 +14010,6 @@
           <t>LL1143</t>
         </is>
       </c>
-      <c r="L213" s="0" t="inlineStr"/>
-      <c r="M213" s="0" t="inlineStr"/>
-      <c r="N213" s="0" t="inlineStr"/>
       <c r="Q213" s="0" t="inlineStr">
         <is>
           <t>M0355</t>
@@ -14425,9 +14078,6 @@
           <t>LL1143</t>
         </is>
       </c>
-      <c r="L214" s="0" t="inlineStr"/>
-      <c r="M214" s="0" t="inlineStr"/>
-      <c r="N214" s="0" t="inlineStr"/>
       <c r="P214" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 6, page 22</t>
@@ -14496,10 +14146,6 @@
           <t>LL1143</t>
         </is>
       </c>
-      <c r="I215" s="0" t="inlineStr"/>
-      <c r="K215" s="0" t="inlineStr"/>
-      <c r="L215" s="0" t="inlineStr"/>
-      <c r="N215" s="0" t="inlineStr"/>
       <c r="P215" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 6, page 22</t>
@@ -14510,7 +14156,6 @@
           <t>colony #2 from M0353 (aka LL1143) serum bottle B, high ethanol production</t>
         </is>
       </c>
-      <c r="S215" s="0" t="inlineStr"/>
       <c r="T215" s="0" t="inlineStr">
         <is>
           <t>LL1143  ∆pyrF ∆(pta-ack) ∆ldh_x000d_
@@ -14546,7 +14191,6 @@
       <c r="C216" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D216" s="0" t="inlineStr"/>
       <c r="E216" s="0" t="b">
         <v>0</v>
       </c>
@@ -14565,10 +14209,6 @@
           <t>LL1143</t>
         </is>
       </c>
-      <c r="I216" s="0" t="inlineStr"/>
-      <c r="K216" s="0" t="inlineStr"/>
-      <c r="L216" s="0" t="inlineStr"/>
-      <c r="N216" s="0" t="inlineStr"/>
       <c r="P216" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 6, page 22</t>
@@ -14579,7 +14219,6 @@
           <t>colony #3 from M0353 (aka LL1143) serum bottle C,  low ethanol production</t>
         </is>
       </c>
-      <c r="S216" s="0" t="inlineStr"/>
       <c r="T216" s="0" t="inlineStr">
         <is>
           <t>LL1143  ∆pyrF ∆(pta-ack) ∆ldh_x000d_
@@ -14633,9 +14272,6 @@
           <t>LL1143</t>
         </is>
       </c>
-      <c r="L217" s="0" t="inlineStr"/>
-      <c r="M217" s="0" t="inlineStr"/>
-      <c r="N217" s="0" t="inlineStr"/>
       <c r="P217" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 6, page 22</t>
@@ -14646,7 +14282,6 @@
           <t>colony #4 from M0353 (aka LL1143) tube B, low ethanol production</t>
         </is>
       </c>
-      <c r="S217" s="0" t="inlineStr"/>
       <c r="T217" s="0" t="inlineStr">
         <is>
           <t>LL1143  ∆pyrF ∆(pta-ack) ∆ldh_x000d_
@@ -14682,7 +14317,6 @@
       <c r="C218" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D218" s="0" t="inlineStr"/>
       <c r="E218" s="0" t="b">
         <v>0</v>
       </c>
@@ -14701,11 +14335,6 @@
           <t>LL1141</t>
         </is>
       </c>
-      <c r="L218" s="0" t="inlineStr"/>
-      <c r="M218" s="0" t="inlineStr"/>
-      <c r="N218" s="0" t="inlineStr"/>
-      <c r="P218" s="0" t="inlineStr"/>
-      <c r="Q218" s="0" t="inlineStr"/>
       <c r="R218" s="0" t="inlineStr">
         <is>
           <t>pfl and pfor deletion in T. sacch</t>
@@ -14758,7 +14387,6 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H219" s="0" t="inlineStr"/>
       <c r="K219" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -14799,7 +14427,6 @@
           <t> ∆ldh::erm ∆(pta-ack)::kan</t>
         </is>
       </c>
-      <c r="T219" s="0" t="inlineStr"/>
       <c r="U219" s="0" t="b">
         <v>0</v>
       </c>
@@ -14834,8 +14461,6 @@
           <t>Kluyveromyces marxianus</t>
         </is>
       </c>
-      <c r="H220" s="0" t="inlineStr"/>
-      <c r="K220" s="0" t="inlineStr"/>
       <c r="L220" s="0" t="inlineStr">
         <is>
           <t>YPD</t>
@@ -14851,15 +14476,11 @@
           <t>glucose</t>
         </is>
       </c>
-      <c r="P220" s="0" t="inlineStr"/>
-      <c r="Q220" s="0" t="inlineStr"/>
       <c r="R220" s="0" t="inlineStr">
         <is>
           <t>Yeast strain purchased from ATCC, 26548</t>
         </is>
       </c>
-      <c r="S220" s="0" t="inlineStr"/>
-      <c r="T220" s="0" t="inlineStr"/>
       <c r="U220" s="0" t="b">
         <v>0</v>
       </c>
@@ -14894,8 +14515,6 @@
           <t>Ogataea polymorpha</t>
         </is>
       </c>
-      <c r="H221" s="0" t="inlineStr"/>
-      <c r="K221" s="0" t="inlineStr"/>
       <c r="L221" s="0" t="inlineStr">
         <is>
           <t>YPD</t>
@@ -14911,14 +14530,11 @@
           <t>glucose</t>
         </is>
       </c>
-      <c r="P221" s="0" t="inlineStr"/>
-      <c r="Q221" s="0" t="inlineStr"/>
       <c r="R221" s="0" t="inlineStr">
         <is>
           <t>Yeast strain purchased from ATCC, 14754.</t>
         </is>
       </c>
-      <c r="T221" s="0" t="inlineStr"/>
       <c r="U221" s="0" t="b">
         <v>0</v>
       </c>
@@ -14973,7 +14589,6 @@
           <t>MTC-5</t>
         </is>
       </c>
-      <c r="M222" s="0" t="inlineStr"/>
       <c r="N222" s="0" t="inlineStr">
         <is>
           <t>Tm6</t>
@@ -14985,7 +14600,6 @@
 SH book III, p. 85 - reference fermentation summary page</t>
         </is>
       </c>
-      <c r="Q222" s="0" t="inlineStr"/>
       <c r="R222" s="0" t="inlineStr">
         <is>
           <t>TC166-1, similar to LL1183, but makes more ethanol.  C. therm adhE driven by enolase promoter on pDGO113.</t>
@@ -15063,7 +14677,6 @@
           <t>MTC-5</t>
         </is>
       </c>
-      <c r="M223" s="0" t="inlineStr"/>
       <c r="N223" s="0" t="inlineStr">
         <is>
           <t>Tm6</t>
@@ -15074,7 +14687,6 @@
           <t>SH Book III Pg 32, 50 – transformation and colony screening, SH Book III Pg 85 – reference fermentation summary page</t>
         </is>
       </c>
-      <c r="Q223" s="0" t="inlineStr"/>
       <c r="R223" s="0" t="inlineStr">
         <is>
           <t>TC166-2, similar to LL1182, but makes less ethanol.  Based on JGI sequence data, plasmid does not seem to be present.  No adhE either.</t>
@@ -15132,7 +14744,6 @@
           <t>LL1070</t>
         </is>
       </c>
-      <c r="K224" s="0" t="inlineStr"/>
       <c r="L224" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -15148,8 +14759,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P224" s="0" t="inlineStr"/>
-      <c r="Q224" s="0" t="inlineStr"/>
       <c r="R224" s="0" t="inlineStr">
         <is>
           <t>AG553 from Adam Guss, strain sent by Beth Papanek.  Might be the same as strain LL1039 and LL1199.  I'm not 100% sure that LL1070 is the parent strain.</t>
@@ -15214,7 +14823,6 @@
           <t>LL1146</t>
         </is>
       </c>
-      <c r="K225" s="0" t="inlineStr"/>
       <c r="L225" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -15530,7 +15138,6 @@
       <c r="C229" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D229" s="0" t="inlineStr"/>
       <c r="E229" s="0" t="b">
         <v>0</v>
       </c>
@@ -15584,7 +15191,6 @@
           <t>M2204, hfs*::kan.  T. sacch with hfs point mutation from ethanologen strain re-introduced.</t>
         </is>
       </c>
-      <c r="S229" s="0" t="inlineStr"/>
       <c r="T229" s="0" t="inlineStr">
         <is>
           <t>LL1025 _x000d_
@@ -15612,7 +15218,6 @@
       <c r="C230" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D230" s="0" t="inlineStr"/>
       <c r="E230" s="0" t="b">
         <v>0</v>
       </c>
@@ -15752,7 +15357,6 @@
           <t>M0416, HK06 from Joe Shaw paper, "Identification of FeFe-hydrogenase…"  Deletion of hfs and hydA in T. sacch</t>
         </is>
       </c>
-      <c r="S231" s="0" t="inlineStr"/>
       <c r="T231" s="0" t="inlineStr">
         <is>
           <t>LL1187  Δhfs::kan_x000d_
@@ -15834,7 +15438,6 @@
           <t>M0229, ΔpyrF</t>
         </is>
       </c>
-      <c r="S232" s="0" t="inlineStr"/>
       <c r="T232" s="0" t="inlineStr">
         <is>
           <t>LL1025 _x000d_
@@ -16214,7 +15817,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="N237" s="0" t="inlineStr"/>
       <c r="P237" s="0" t="inlineStr">
         <is>
           <t>SH Book IV, p. 73-92 - transformation and colony screening_x000d_
@@ -16445,14 +16047,6 @@
           <t>Jilai Zhou</t>
         </is>
       </c>
-      <c r="G240" s="0" t="inlineStr"/>
-      <c r="H240" s="0" t="inlineStr"/>
-      <c r="L240" s="0" t="inlineStr"/>
-      <c r="M240" s="0" t="inlineStr"/>
-      <c r="N240" s="0" t="inlineStr"/>
-      <c r="R240" s="0" t="inlineStr"/>
-      <c r="S240" s="0" t="inlineStr"/>
-      <c r="T240" s="0" t="inlineStr"/>
       <c r="U240" s="0" t="b">
         <v>0</v>
       </c>
@@ -16503,7 +16097,6 @@
       <c r="C242" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="D242" s="0" t="inlineStr"/>
       <c r="E242" s="0" t="b">
         <v>0</v>
       </c>
@@ -16512,16 +16105,6 @@
           <t>Jilai Zhou</t>
         </is>
       </c>
-      <c r="G242" s="0" t="inlineStr"/>
-      <c r="H242" s="0" t="inlineStr"/>
-      <c r="K242" s="0" t="inlineStr"/>
-      <c r="L242" s="0" t="inlineStr"/>
-      <c r="M242" s="0" t="inlineStr"/>
-      <c r="N242" s="0" t="inlineStr"/>
-      <c r="P242" s="0" t="inlineStr"/>
-      <c r="R242" s="0" t="inlineStr"/>
-      <c r="S242" s="0" t="inlineStr"/>
-      <c r="T242" s="0" t="inlineStr"/>
       <c r="U242" s="0" t="b">
         <v>0</v>
       </c>
@@ -16543,7 +16126,6 @@
       <c r="C243" s="0" t="b">
         <v>1</v>
       </c>
-      <c r="D243" s="0" t="inlineStr"/>
       <c r="E243" s="0" t="b">
         <v>0</v>
       </c>
@@ -16552,16 +16134,6 @@
           <t>Jilai Zhou</t>
         </is>
       </c>
-      <c r="G243" s="0" t="inlineStr"/>
-      <c r="H243" s="0" t="inlineStr"/>
-      <c r="K243" s="0" t="inlineStr"/>
-      <c r="L243" s="0" t="inlineStr"/>
-      <c r="M243" s="0" t="inlineStr"/>
-      <c r="N243" s="0" t="inlineStr"/>
-      <c r="P243" s="0" t="inlineStr"/>
-      <c r="R243" s="0" t="inlineStr"/>
-      <c r="S243" s="0" t="inlineStr"/>
-      <c r="T243" s="0" t="inlineStr"/>
       <c r="U243" s="0" t="b">
         <v>0</v>
       </c>
@@ -16601,7 +16173,6 @@
           <t>LL1115</t>
         </is>
       </c>
-      <c r="K244" s="0" t="inlineStr"/>
       <c r="L244" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -16617,13 +16188,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P244" s="0" t="inlineStr"/>
       <c r="R244" s="0" t="inlineStr">
         <is>
           <t>Wild type JW200. Note, this is the same as strain LL1115</t>
         </is>
       </c>
-      <c r="S244" s="0" t="inlineStr"/>
       <c r="T244" s="0" t="inlineStr">
         <is>
           <t>LL1115 _x000d_
@@ -16684,7 +16253,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P245" s="0" t="inlineStr"/>
       <c r="R245" s="0" t="inlineStr">
         <is>
           <t>x5</t>
@@ -16741,7 +16309,6 @@
           <t>LL1204</t>
         </is>
       </c>
-      <c r="K246" s="0" t="inlineStr"/>
       <c r="L246" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -16757,7 +16324,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P246" s="0" t="inlineStr"/>
       <c r="R246" s="0" t="inlineStr">
         <is>
           <t>x6</t>
@@ -16814,7 +16380,6 @@
           <t>LL1204</t>
         </is>
       </c>
-      <c r="K247" s="0" t="inlineStr"/>
       <c r="L247" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -16830,7 +16395,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P247" s="0" t="inlineStr"/>
       <c r="R247" s="0" t="inlineStr">
         <is>
           <t>x7</t>
@@ -16877,14 +16441,6 @@
           <t>Jilai Zhou</t>
         </is>
       </c>
-      <c r="G248" s="0" t="inlineStr"/>
-      <c r="H248" s="0" t="inlineStr"/>
-      <c r="L248" s="0" t="inlineStr"/>
-      <c r="M248" s="0" t="inlineStr"/>
-      <c r="N248" s="0" t="inlineStr"/>
-      <c r="R248" s="0" t="inlineStr"/>
-      <c r="S248" s="0" t="inlineStr"/>
-      <c r="T248" s="0" t="inlineStr"/>
       <c r="U248" s="0" t="b">
         <v>0</v>
       </c>
@@ -17111,7 +16667,6 @@
           <t>LL1010</t>
         </is>
       </c>
-      <c r="I251" s="0" t="inlineStr"/>
       <c r="K251" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -17194,8 +16749,6 @@
           <t>LL1185</t>
         </is>
       </c>
-      <c r="I252" s="0" t="inlineStr"/>
-      <c r="K252" s="0" t="inlineStr"/>
       <c r="L252" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -17221,7 +16774,6 @@
           <t>Strain LL1185 was found to have a bit of wild type contamination after JGI resequencing.  Not sure where the contamination may have occurred, so we colony-purified the strain.</t>
         </is>
       </c>
-      <c r="S252" s="0" t="inlineStr"/>
       <c r="T252" s="0" t="inlineStr">
         <is>
           <t>LL1185  ∆pyrF ∆(pta-ack)_x000d_
@@ -17269,7 +16821,6 @@
           <t>LL1163</t>
         </is>
       </c>
-      <c r="I253" s="0" t="inlineStr"/>
       <c r="K253" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -17355,7 +16906,6 @@
           <t>LL1163</t>
         </is>
       </c>
-      <c r="I254" s="0" t="inlineStr"/>
       <c r="K254" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -17441,7 +16991,6 @@
           <t>LL1205</t>
         </is>
       </c>
-      <c r="I255" s="0" t="inlineStr"/>
       <c r="L255" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -17457,7 +17006,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P255" s="0" t="inlineStr"/>
       <c r="R255" s="0" t="inlineStr">
         <is>
           <t>x8, JS044, ΔadhA::Kan ΔadhB::Tm</t>
@@ -17515,7 +17063,6 @@
           <t>LL1206</t>
         </is>
       </c>
-      <c r="I256" s="0" t="inlineStr"/>
       <c r="L256" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -17531,7 +17078,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P256" s="0" t="inlineStr"/>
       <c r="R256" s="0" t="inlineStr">
         <is>
           <t>x9, JS045, ΔadhB::Kan ΔadhE::Tm</t>
@@ -17589,7 +17135,6 @@
           <t>LL1207</t>
         </is>
       </c>
-      <c r="I257" s="0" t="inlineStr"/>
       <c r="L257" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -17605,7 +17150,6 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P257" s="0" t="inlineStr"/>
       <c r="R257" s="0" t="inlineStr">
         <is>
           <t>x10, JS046, ΔadhE::Kan ΔadhA::Tm</t>
@@ -17737,7 +17281,6 @@
       <c r="C259" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D259" s="0" t="inlineStr"/>
       <c r="E259" s="0" t="b">
         <v>0</v>
       </c>
@@ -17834,7 +17377,6 @@
       <c r="C260" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D260" s="0" t="inlineStr"/>
       <c r="E260" s="0" t="b">
         <v>0</v>
       </c>
@@ -17993,7 +17535,6 @@
           <t>J Lo Lab notebook 7, page 5-6</t>
         </is>
       </c>
-      <c r="R262" s="0" t="inlineStr"/>
       <c r="S262" s="0" t="inlineStr">
         <is>
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure ure metE Δeps ΔnfnAB::kan xynA::nfnAB erm</t>
@@ -18050,16 +17591,11 @@
           <t>TOPO PxynA::nfnAB::erm</t>
         </is>
       </c>
-      <c r="K263" s="0" t="inlineStr"/>
-      <c r="L263" s="0" t="inlineStr"/>
-      <c r="M263" s="0" t="inlineStr"/>
-      <c r="N263" s="0" t="inlineStr"/>
       <c r="P263" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 7, page 5-6</t>
         </is>
       </c>
-      <c r="R263" s="0" t="inlineStr"/>
       <c r="S263" s="0" t="inlineStr">
         <is>
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure Δeps ΔnfnAB::kan xynA::nfnAB erm</t>
@@ -18116,10 +17652,6 @@
           <t>pJLO26</t>
         </is>
       </c>
-      <c r="K264" s="0" t="inlineStr"/>
-      <c r="L264" s="0" t="inlineStr"/>
-      <c r="M264" s="0" t="inlineStr"/>
-      <c r="N264" s="0" t="inlineStr"/>
       <c r="P264" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 7, page 9</t>
@@ -18186,7 +17718,6 @@
           <t>pJLO28</t>
         </is>
       </c>
-      <c r="O265" s="1"/>
       <c r="P265" s="0" t="inlineStr">
         <is>
           <t>J Lo Lab notebook 7, page 9</t>
@@ -18687,8 +18218,6 @@
           <t>Geobacillus thermoglucosidasius ATCC 43742</t>
         </is>
       </c>
-      <c r="H272" s="0" t="inlineStr"/>
-      <c r="I272" s="0" t="inlineStr"/>
       <c r="O272" s="1">
         <v>42082</v>
       </c>
@@ -18702,8 +18231,6 @@
           <t>We got this strain to get the adhE for Shuen's paper comparing various different adhEs</t>
         </is>
       </c>
-      <c r="S272" s="0" t="inlineStr"/>
-      <c r="T272" s="0" t="inlineStr"/>
       <c r="U272" s="0" t="b">
         <v>0</v>
       </c>
@@ -18743,7 +18270,6 @@
           <t>LL1197</t>
         </is>
       </c>
-      <c r="I273" s="0" t="inlineStr"/>
       <c r="R273" s="0" t="inlineStr">
         <is>
           <t>Alternative name: TC327A. LL1233 and LL1234 are sister colonies</t>
@@ -18803,8 +18329,6 @@
           <t>LL1197</t>
         </is>
       </c>
-      <c r="O274" s="1"/>
-      <c r="P274" s="0" t="inlineStr"/>
       <c r="R274" s="0" t="inlineStr">
         <is>
           <t>Alternative name: TC327B. LL1233 and LL1234 are sister colonies</t>
@@ -18928,8 +18452,6 @@
           <t>LL1197</t>
         </is>
       </c>
-      <c r="I276" s="0" t="inlineStr"/>
-      <c r="P276" s="0" t="inlineStr"/>
       <c r="R276" s="0" t="inlineStr">
         <is>
           <t>Alternative name: TC328B. LL1235 and LL1236 are sister colonies</t>
@@ -18994,9 +18516,6 @@
           <t>pSH43</t>
         </is>
       </c>
-      <c r="L277" s="0" t="inlineStr"/>
-      <c r="M277" s="0" t="inlineStr"/>
-      <c r="N277" s="0" t="inlineStr"/>
       <c r="R277" s="0" t="inlineStr">
         <is>
           <t>Alternative name: TC329A.  LL1237 and LL1238 are sister colonies.</t>
@@ -19061,11 +18580,6 @@
           <t>pSH43</t>
         </is>
       </c>
-      <c r="K278" s="0" t="inlineStr"/>
-      <c r="L278" s="0" t="inlineStr"/>
-      <c r="M278" s="0" t="inlineStr"/>
-      <c r="N278" s="0" t="inlineStr"/>
-      <c r="P278" s="0" t="inlineStr"/>
       <c r="R278" s="0" t="inlineStr">
         <is>
           <t>Alternative name: TC329B.  LL1237 and LL1238 are sister colonies.</t>
@@ -19107,7 +18621,6 @@
       <c r="C279" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D279" s="0" t="inlineStr"/>
       <c r="E279" s="0" t="b">
         <v>0</v>
       </c>
@@ -19131,11 +18644,6 @@
           <t>pSH44</t>
         </is>
       </c>
-      <c r="K279" s="0" t="inlineStr"/>
-      <c r="L279" s="0" t="inlineStr"/>
-      <c r="M279" s="0" t="inlineStr"/>
-      <c r="N279" s="0" t="inlineStr"/>
-      <c r="P279" s="0" t="inlineStr"/>
       <c r="R279" s="0" t="inlineStr">
         <is>
           <t>Alternative name: TC330A.  LL1239 and LL1240 are sister colonies.</t>
@@ -19200,11 +18708,6 @@
           <t>pSH44</t>
         </is>
       </c>
-      <c r="K280" s="0" t="inlineStr"/>
-      <c r="L280" s="0" t="inlineStr"/>
-      <c r="M280" s="0" t="inlineStr"/>
-      <c r="N280" s="0" t="inlineStr"/>
-      <c r="P280" s="0" t="inlineStr"/>
       <c r="R280" s="0" t="inlineStr">
         <is>
           <t>Alternative name: TC330B.  LL1239 and LL1240 are sister colonies.</t>
@@ -19259,12 +18762,6 @@
           <t>Clostridium kluyveri DSM 555</t>
         </is>
       </c>
-      <c r="H281" s="0" t="inlineStr"/>
-      <c r="I281" s="0" t="inlineStr"/>
-      <c r="K281" s="0" t="inlineStr"/>
-      <c r="L281" s="0" t="inlineStr"/>
-      <c r="M281" s="0" t="inlineStr"/>
-      <c r="N281" s="0" t="inlineStr"/>
       <c r="O281" s="1">
         <v>42082</v>
       </c>
@@ -19278,8 +18775,6 @@
           <t>Shuen got it from Jon Lo.  Jon got it to use as a control for nfnAB assays.  I think this is the ATCC strain, which is the same as LL1307.</t>
         </is>
       </c>
-      <c r="S281" s="0" t="inlineStr"/>
-      <c r="T281" s="0" t="inlineStr"/>
       <c r="U281" s="0" t="b">
         <v>0</v>
       </c>
@@ -19319,7 +18814,6 @@
           <t>LL1199</t>
         </is>
       </c>
-      <c r="P282" s="0" t="inlineStr"/>
       <c r="R282" s="0" t="inlineStr">
         <is>
           <t>Evolved from LL1199.  Very similar ethanol production to LL1230 (also similar by sequencing data).</t>
@@ -19445,7 +18939,6 @@
           <t>Thermoanaerobacterium thermosaccharolyticum DSM 571</t>
         </is>
       </c>
-      <c r="H284" s="0" t="inlineStr"/>
       <c r="L284" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -19461,14 +18954,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P284" s="0" t="inlineStr"/>
       <c r="R284" s="0" t="inlineStr">
         <is>
           <t>from Mascoma: filed by Joe Shaw M1290, ATCC 31960 the HG-8 substrain from DSM 571</t>
         </is>
       </c>
-      <c r="S284" s="0" t="inlineStr"/>
-      <c r="T284" s="0" t="inlineStr"/>
       <c r="U284" s="0" t="b">
         <v>0</v>
       </c>
@@ -19936,13 +19426,11 @@
           <t>Escherichia coli</t>
         </is>
       </c>
-      <c r="H290" s="0" t="inlineStr"/>
       <c r="R290" s="0" t="inlineStr">
         <is>
           <t>FF50.  Pyruvate kinase deletion strain of E. coli from Aron Fenton.   Ishwar A, Tang Q, Fenton AW: Distinguishing the Interactions in the Fructose 1,6-Bisphosphate Binding Site of Human Liver Pyruvate Kinase That Contribute to Allostery. Biochemistry 20</t>
         </is>
       </c>
-      <c r="T290" s="0" t="inlineStr"/>
       <c r="U290" s="0" t="b">
         <v>0</v>
       </c>
@@ -20045,7 +19533,6 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="H292" s="0" t="inlineStr"/>
       <c r="R292" s="0" t="inlineStr">
         <is>
           <t>mdh deletion strain from Paul Lin, PhD student in Jim Liao's lab at UCLA.  I think it was created in a wild-type background.  Plasmid pPL100_Dmdh was used.  This plasmid leaves the gapD-cat marker on the genome.  There are cre-lox sites that can be used f</t>
@@ -20056,7 +19543,6 @@
           <t> Δhpt Δmdh</t>
         </is>
       </c>
-      <c r="T292" s="0" t="inlineStr"/>
       <c r="U292" s="0" t="b">
         <v>0</v>
       </c>
@@ -20333,8 +19819,6 @@
           <t>LL1206</t>
         </is>
       </c>
-      <c r="R297" s="0" t="inlineStr"/>
-      <c r="S297" s="0" t="inlineStr"/>
       <c r="T297" s="0" t="inlineStr">
         <is>
           <t>LL1206  ΔadhB::kan_x000d_
@@ -20377,14 +19861,11 @@
           <t>Thermoanaerobacter mathranii</t>
         </is>
       </c>
-      <c r="H298" s="0" t="inlineStr"/>
       <c r="R298" s="0" t="inlineStr">
         <is>
           <t>Strain DSM 11426, via Xiongjun Shao</t>
         </is>
       </c>
-      <c r="S298" s="0" t="inlineStr"/>
-      <c r="T298" s="0" t="inlineStr"/>
       <c r="U298" s="0" t="b">
         <v>0</v>
       </c>
@@ -20424,10 +19905,6 @@
           <t>LL1260</t>
         </is>
       </c>
-      <c r="L299" s="0" t="inlineStr"/>
-      <c r="M299" s="0" t="inlineStr"/>
-      <c r="N299" s="0" t="inlineStr"/>
-      <c r="P299" s="0" t="inlineStr"/>
       <c r="R299" s="0" t="inlineStr">
         <is>
           <t>Intermediate strain between LL1149 and LL1210, evolved 1 month after LL1260._x000d_
@@ -20493,10 +19970,6 @@
           <t>LL1149</t>
         </is>
       </c>
-      <c r="L300" s="0" t="inlineStr"/>
-      <c r="M300" s="0" t="inlineStr"/>
-      <c r="N300" s="0" t="inlineStr"/>
-      <c r="P300" s="0" t="inlineStr"/>
       <c r="R300" s="0" t="inlineStr">
         <is>
           <t>Intermediate strain between LL1149 and LL1210, evolved 1 month after LL1149._x000d_
@@ -20561,10 +20034,6 @@
           <t>LL1259</t>
         </is>
       </c>
-      <c r="L301" s="0" t="inlineStr"/>
-      <c r="M301" s="0" t="inlineStr"/>
-      <c r="N301" s="0" t="inlineStr"/>
-      <c r="P301" s="0" t="inlineStr"/>
       <c r="R301" s="0" t="inlineStr">
         <is>
           <t>Intermediate strain between LL1149 and LL1210, evolved 1 month after LL1259._x000d_
@@ -20631,10 +20100,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="L302" s="0" t="inlineStr"/>
-      <c r="M302" s="0" t="inlineStr"/>
-      <c r="N302" s="0" t="inlineStr"/>
-      <c r="P302" s="0" t="inlineStr"/>
       <c r="R302" s="0" t="inlineStr">
         <is>
           <t>LL345 with Clo1313_0099 deletion, acetolactate synthase.  Liang thinks this might not be the right acetolactate synthase.</t>
@@ -20691,10 +20156,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="L303" s="0" t="inlineStr"/>
-      <c r="M303" s="0" t="inlineStr"/>
-      <c r="N303" s="0" t="inlineStr"/>
-      <c r="P303" s="0" t="inlineStr"/>
       <c r="R303" s="0" t="inlineStr">
         <is>
           <t>LL345 with Clo1313_0099 deletion, sister colony to LL1262</t>
@@ -20751,7 +20212,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="P304" s="0" t="inlineStr"/>
       <c r="R304" s="0" t="inlineStr">
         <is>
           <t>LL345 with Clo1313_0099 deletion, sister colony to LL1262.</t>
@@ -20808,7 +20268,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="P305" s="0" t="inlineStr"/>
       <c r="R305" s="0" t="inlineStr">
         <is>
           <t>LL345 with Clo1313_0099 deletion, sister colony to LL1262</t>
@@ -20829,8 +20288,6 @@
       <c r="U305" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W305" s="0" t="inlineStr"/>
-      <c r="X305" s="0" t="inlineStr"/>
       <c r="Y305" s="0" t="inlineStr">
         <is>
           <t>1265</t>
@@ -20862,7 +20319,6 @@
           <t>Thermoanaerobacter ethanolicus ATCC 31550</t>
         </is>
       </c>
-      <c r="H306" s="0" t="inlineStr"/>
       <c r="L306" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -20883,14 +20339,9 @@
           <t>Xiongjun notebook #3</t>
         </is>
       </c>
-      <c r="R306" s="0" t="inlineStr"/>
-      <c r="S306" s="0" t="inlineStr"/>
-      <c r="T306" s="0" t="inlineStr"/>
       <c r="U306" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W306" s="0" t="inlineStr"/>
-      <c r="X306" s="0" t="inlineStr"/>
       <c r="Y306" s="0" t="inlineStr">
         <is>
           <t>1266</t>
@@ -21041,8 +20492,6 @@
       <c r="U308" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W308" s="0" t="inlineStr"/>
-      <c r="X308" s="0" t="inlineStr"/>
       <c r="Y308" s="0" t="inlineStr">
         <is>
           <t>1268</t>
@@ -21118,8 +20567,6 @@
       <c r="U309" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W309" s="0" t="inlineStr"/>
-      <c r="X309" s="0" t="inlineStr"/>
       <c r="Y309" s="0" t="inlineStr">
         <is>
           <t>1269</t>
@@ -21195,8 +20642,6 @@
       <c r="U310" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W310" s="0" t="inlineStr"/>
-      <c r="X310" s="0" t="inlineStr"/>
       <c r="Y310" s="0" t="inlineStr">
         <is>
           <t>1270</t>
@@ -21369,10 +20814,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="K313" s="0" t="inlineStr"/>
-      <c r="L313" s="0" t="inlineStr"/>
-      <c r="M313" s="0" t="inlineStr"/>
-      <c r="N313" s="0" t="inlineStr"/>
       <c r="P313" s="0" t="inlineStr">
         <is>
           <t>Jon Lo, notebook 7 p. 20-22</t>
@@ -21446,10 +20887,6 @@
           <t>LL350</t>
         </is>
       </c>
-      <c r="K314" s="0" t="inlineStr"/>
-      <c r="L314" s="0" t="inlineStr"/>
-      <c r="M314" s="0" t="inlineStr"/>
-      <c r="N314" s="0" t="inlineStr"/>
       <c r="P314" s="0" t="inlineStr">
         <is>
           <t>Jon Lo, notebook 7 p. 20-22</t>
@@ -21514,10 +20951,6 @@
           <t>LL350</t>
         </is>
       </c>
-      <c r="K315" s="0" t="inlineStr"/>
-      <c r="L315" s="0" t="inlineStr"/>
-      <c r="M315" s="0" t="inlineStr"/>
-      <c r="N315" s="0" t="inlineStr"/>
       <c r="P315" s="0" t="inlineStr">
         <is>
           <t>Jon Lo, notebook 7 p. 20-22</t>
@@ -21592,10 +21025,6 @@
           <t>LL350</t>
         </is>
       </c>
-      <c r="K316" s="0" t="inlineStr"/>
-      <c r="L316" s="0" t="inlineStr"/>
-      <c r="M316" s="0" t="inlineStr"/>
-      <c r="N316" s="0" t="inlineStr"/>
       <c r="P316" s="0" t="inlineStr">
         <is>
           <t>Jon Lo, notebook 7 p. 20-22</t>
@@ -21670,10 +21099,6 @@
           <t>LL1147</t>
         </is>
       </c>
-      <c r="K317" s="0" t="inlineStr"/>
-      <c r="L317" s="0" t="inlineStr"/>
-      <c r="M317" s="0" t="inlineStr"/>
-      <c r="N317" s="0" t="inlineStr"/>
       <c r="P317" s="0" t="inlineStr">
         <is>
           <t>Jon Lo, notebook 7 p. 20-22</t>
@@ -21749,10 +21174,6 @@
           <t>LL1163</t>
         </is>
       </c>
-      <c r="K318" s="0" t="inlineStr"/>
-      <c r="L318" s="0" t="inlineStr"/>
-      <c r="M318" s="0" t="inlineStr"/>
-      <c r="N318" s="0" t="inlineStr"/>
       <c r="P318" s="0" t="inlineStr">
         <is>
           <t>Jon Lo, notebook 7 p. 20-22</t>
@@ -21820,10 +21241,6 @@
           <t>LL1163</t>
         </is>
       </c>
-      <c r="K319" s="0" t="inlineStr"/>
-      <c r="L319" s="0" t="inlineStr"/>
-      <c r="M319" s="0" t="inlineStr"/>
-      <c r="N319" s="0" t="inlineStr"/>
       <c r="P319" s="0" t="inlineStr">
         <is>
           <t>Jon Lo, notebook 7 p. 20-22</t>
@@ -22291,7 +21708,6 @@
           <t>LL1049</t>
         </is>
       </c>
-      <c r="I325" s="0" t="inlineStr"/>
       <c r="K325" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -22372,7 +21788,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="I326" s="0" t="inlineStr"/>
       <c r="K326" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -22453,7 +21868,6 @@
           <t>LL1049</t>
         </is>
       </c>
-      <c r="I327" s="0" t="inlineStr"/>
       <c r="K327" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -22534,7 +21948,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="I328" s="0" t="inlineStr"/>
       <c r="K328" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -22615,7 +22028,6 @@
           <t>LL1049</t>
         </is>
       </c>
-      <c r="I329" s="0" t="inlineStr"/>
       <c r="K329" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -22871,7 +22283,6 @@
           <t>WT + complete T. sacch EtOH pathway (adhE, nfnAB and adhA), strain 478-3</t>
         </is>
       </c>
-      <c r="S332" s="0" t="inlineStr"/>
       <c r="T332" s="0" t="inlineStr">
         <is>
           <t>LL1004 _x000d_
@@ -23347,11 +22758,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="K339" s="0" t="inlineStr"/>
-      <c r="L339" s="0" t="inlineStr"/>
-      <c r="M339" s="0" t="inlineStr"/>
-      <c r="N339" s="0" t="inlineStr"/>
-      <c r="P339" s="0" t="inlineStr"/>
       <c r="R339" s="0" t="inlineStr">
         <is>
           <t>Adam Guss strain AG929.  Restriction enzyme deletion, Clo1313_0478.  Created by Beth Papanek in Adam Guss's lab at ORNL.  See email from Beth Papanek to Dan Olson regarding strain transfer on Nov. 10th, 2015.</t>
@@ -23403,9 +22809,6 @@
           <t>Thermoanaerobacter brockii subsp finii</t>
         </is>
       </c>
-      <c r="L340" s="0" t="inlineStr"/>
-      <c r="M340" s="0" t="inlineStr"/>
-      <c r="N340" s="0" t="inlineStr"/>
       <c r="R340" s="0" t="inlineStr">
         <is>
           <t>DSMZ 3389, Mascoma strain M32 or M0032</t>
@@ -23445,9 +22848,6 @@
           <t>Thermoanaerobacterium xylanolyticum</t>
         </is>
       </c>
-      <c r="L341" s="0" t="inlineStr"/>
-      <c r="M341" s="0" t="inlineStr"/>
-      <c r="N341" s="0" t="inlineStr"/>
       <c r="R341" s="0" t="inlineStr">
         <is>
           <t>DSMZ 7097, Mascoma strain M26 or M0026</t>
@@ -23487,13 +22887,11 @@
           <t>Bacteroides cellulosilyticus</t>
         </is>
       </c>
-      <c r="H342" s="0" t="inlineStr"/>
       <c r="R342" s="0" t="inlineStr">
         <is>
           <t>Strain WH2.  Grow at 37C anaerobically on CTFUD at pH 7.2 supplemented with 1 µg/ml vitamin K3 dissolved in ethanol, 0.005 µg/ml vitamin B12 in water and 1.2 µg/ml hematin + 0.2 mM L-histidine pH 8.0.  This strain grows on arabinoxylan.</t>
         </is>
       </c>
-      <c r="T342" s="0" t="inlineStr"/>
       <c r="U342" s="0" t="b">
         <v>0</v>
       </c>
@@ -23528,13 +22926,11 @@
           <t>Bacteroides cellulosilyticus</t>
         </is>
       </c>
-      <c r="H343" s="0" t="inlineStr"/>
       <c r="R343" s="0" t="inlineStr">
         <is>
           <t>Strain DSM 14838.  Grow at 37C anaerobically on CTFUD at pH 7.2 supplemented with 1 µg/ml vitamin K3 dissolved in ethanol, 0.005 µg/ml vitamin B12 in water and 1.2 µg/ml hematin + 0.2 mM L-histidine pH 8.0.  This strain grows on arabinoxylan.</t>
         </is>
       </c>
-      <c r="T343" s="0" t="inlineStr"/>
       <c r="U343" s="0" t="b">
         <v>0</v>
       </c>
@@ -23630,7 +23026,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="I345" s="0" t="inlineStr"/>
       <c r="K345" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -23711,7 +23106,6 @@
           <t>LL1305</t>
         </is>
       </c>
-      <c r="I346" s="0" t="inlineStr"/>
       <c r="K346" s="0" t="inlineStr">
         <is>
           <t>20% glycerol, 30% water, 50% culture</t>
@@ -23783,8 +23177,6 @@
           <t>Clostridium kluyveri DSM 555</t>
         </is>
       </c>
-      <c r="H347" s="0" t="inlineStr"/>
-      <c r="I347" s="0" t="inlineStr"/>
       <c r="L347" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -23800,14 +23192,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P347" s="0" t="inlineStr"/>
       <c r="R347" s="0" t="inlineStr">
         <is>
           <t>Clostridium kluyveri DSM555, from ATCC</t>
         </is>
       </c>
-      <c r="S347" s="0" t="inlineStr"/>
-      <c r="T347" s="0" t="inlineStr"/>
       <c r="U347" s="0" t="b">
         <v>0</v>
       </c>
@@ -23837,9 +23226,6 @@
           <t>Chris Herring</t>
         </is>
       </c>
-      <c r="G348" s="0" t="inlineStr"/>
-      <c r="H348" s="0" t="inlineStr"/>
-      <c r="I348" s="0" t="inlineStr"/>
       <c r="L348" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -23855,14 +23241,11 @@
           <t>cellobiose</t>
         </is>
       </c>
-      <c r="P348" s="0" t="inlineStr"/>
       <c r="R348" s="0" t="inlineStr">
         <is>
           <t>M1059 (from Mascoma, I think)</t>
         </is>
       </c>
-      <c r="S348" s="0" t="inlineStr"/>
-      <c r="T348" s="0" t="inlineStr"/>
       <c r="U348" s="0" t="b">
         <v>0</v>
       </c>
@@ -24089,8 +23472,6 @@
           <t>pLL1143</t>
         </is>
       </c>
-      <c r="L352" s="0" t="inlineStr"/>
-      <c r="O352" s="1"/>
       <c r="P352" s="0" t="inlineStr">
         <is>
           <t>MM17 p. 5</t>
@@ -24146,14 +23527,11 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="H353" s="0" t="inlineStr"/>
       <c r="I353" s="0" t="inlineStr">
         <is>
           <t>pLL1143</t>
         </is>
       </c>
-      <c r="L353" s="0" t="inlineStr"/>
-      <c r="O353" s="1"/>
       <c r="P353" s="0" t="inlineStr">
         <is>
           <t>MM17 p. 5</t>
@@ -24164,8 +23542,6 @@
           <t>MM30 #8 Clo1313_0076 adh attempted deletion.  Marybeth tried to grow this strain, but it didn't grow.  Strain is presumed lost.</t>
         </is>
       </c>
-      <c r="S353" s="0" t="inlineStr"/>
-      <c r="T353" s="0" t="inlineStr"/>
       <c r="U353" s="0" t="b">
         <v>0</v>
       </c>
@@ -24210,8 +23586,6 @@
           <t>pLL1145</t>
         </is>
       </c>
-      <c r="L354" s="0" t="inlineStr"/>
-      <c r="O354" s="1"/>
       <c r="P354" s="0" t="inlineStr">
         <is>
           <t>MB notebook 17, p. 5</t>
@@ -24277,8 +23651,6 @@
           <t>pLL1145</t>
         </is>
       </c>
-      <c r="L355" s="0" t="inlineStr"/>
-      <c r="O355" s="1"/>
       <c r="P355" s="0" t="inlineStr">
         <is>
           <t>MB notebook 17, p. 5</t>
@@ -24339,15 +23711,11 @@
           <t>LL1306</t>
         </is>
       </c>
-      <c r="L356" s="0" t="inlineStr"/>
-      <c r="O356" s="1"/>
-      <c r="P356" s="0" t="inlineStr"/>
       <c r="R356" s="0" t="inlineStr">
         <is>
           <t>LL1025 Δtdk ΔTsac_1705 ΔnfnAB</t>
         </is>
       </c>
-      <c r="S356" s="0" t="inlineStr"/>
       <c r="T356" s="0" t="inlineStr">
         <is>
           <t>LL1306 _x000d_
@@ -24395,15 +23763,11 @@
           <t>LL1144</t>
         </is>
       </c>
-      <c r="L357" s="0" t="inlineStr"/>
-      <c r="O357" s="1"/>
-      <c r="P357" s="0" t="inlineStr"/>
       <c r="R357" s="0" t="inlineStr">
         <is>
           <t>LL1025 Δtdk ΔnfnAB::kan</t>
         </is>
       </c>
-      <c r="S357" s="0" t="inlineStr"/>
       <c r="T357" s="0" t="inlineStr">
         <is>
           <t>LL1144  ΔnfnAB::kan_x000d_
@@ -24450,9 +23814,6 @@
           <t>LL1251</t>
         </is>
       </c>
-      <c r="L358" s="0" t="inlineStr"/>
-      <c r="O358" s="1"/>
-      <c r="P358" s="0" t="inlineStr"/>
       <c r="R358" s="0" t="inlineStr">
         <is>
           <t>LL1251 with ech deletion.  According to JGI sequence data, hpt deletion is present, malic enzyme deletion is present, pyk insertion at ldh is present, peps deletion is present, ppdk deletion is present, ech deletion is present.  Strain is correct.</t>
@@ -25097,14 +24458,11 @@
           <t>Clostridium stercorarium</t>
         </is>
       </c>
-      <c r="H367" s="0" t="inlineStr"/>
       <c r="R367" s="0" t="inlineStr">
         <is>
           <t>DSM 8532, grown on DSM medium 255 (Clostridium GS medium) at 60 deg. C</t>
         </is>
       </c>
-      <c r="S367" s="0" t="inlineStr"/>
-      <c r="T367" s="0" t="inlineStr"/>
       <c r="U367" s="0" t="b">
         <v>0</v>
       </c>
@@ -25194,10 +24552,6 @@
           <t>LL1328</t>
         </is>
       </c>
-      <c r="I369" s="0" t="inlineStr"/>
-      <c r="L369" s="0" t="inlineStr"/>
-      <c r="P369" s="0" t="inlineStr"/>
-      <c r="R369" s="0" t="inlineStr"/>
       <c r="S369" s="0" t="inlineStr">
         <is>
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure Δeps Δtdk Δadh0218</t>
@@ -25249,9 +24603,6 @@
           <t>LL1329</t>
         </is>
       </c>
-      <c r="L370" s="0" t="inlineStr"/>
-      <c r="P370" s="0" t="inlineStr"/>
-      <c r="R370" s="0" t="inlineStr"/>
       <c r="S370" s="0" t="inlineStr">
         <is>
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure Δeps Δtdk Δadh0218 Δadh2222</t>
@@ -25304,9 +24655,6 @@
           <t>LL1330</t>
         </is>
       </c>
-      <c r="I371" s="0" t="inlineStr"/>
-      <c r="P371" s="0" t="inlineStr"/>
-      <c r="R371" s="0" t="inlineStr"/>
       <c r="S371" s="0" t="inlineStr">
         <is>
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure Δeps Δtdk Δadh0218 Δadh2222 Δadh0285</t>
@@ -25360,8 +24708,6 @@
           <t>LL1331</t>
         </is>
       </c>
-      <c r="P372" s="0" t="inlineStr"/>
-      <c r="R372" s="0" t="inlineStr"/>
       <c r="S372" s="0" t="inlineStr">
         <is>
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure Δeps Δtdk Δadh0218 Δadh2222 Δadh0285 Δadh1049</t>
@@ -25416,9 +24762,6 @@
           <t>LL1332</t>
         </is>
       </c>
-      <c r="I373" s="0" t="inlineStr"/>
-      <c r="P373" s="0" t="inlineStr"/>
-      <c r="R373" s="0" t="inlineStr"/>
       <c r="S373" s="0" t="inlineStr">
         <is>
           <t> ∆(pta-ack) ∆ldh Δor795::metE-ure Δeps Δtdk Δadh0218 Δadh2222 Δadh0285 Δadh1049 ΔadhA::kan</t>
@@ -25474,8 +24817,6 @@
           <t>LL1076</t>
         </is>
       </c>
-      <c r="I374" s="0" t="inlineStr"/>
-      <c r="P374" s="0" t="inlineStr"/>
       <c r="R374" s="0" t="inlineStr">
         <is>
           <t>LL1076 with the pta-ack cassette removed by counterselection</t>
@@ -25532,9 +24873,6 @@
           <t>LL1334</t>
         </is>
       </c>
-      <c r="I375" s="0" t="inlineStr"/>
-      <c r="P375" s="0" t="inlineStr"/>
-      <c r="R375" s="0" t="inlineStr"/>
       <c r="S375" s="0" t="inlineStr">
         <is>
           <t> ΔadhE ΔadhA::kan</t>
@@ -26119,8 +25457,6 @@
           <t>Dhananjay Beri</t>
         </is>
       </c>
-      <c r="G384" s="0" t="inlineStr"/>
-      <c r="R384" s="0" t="inlineStr"/>
       <c r="U384" s="0" t="b">
         <v>0</v>
       </c>
@@ -26150,11 +25486,6 @@
           <t>Dhananjay Beri</t>
         </is>
       </c>
-      <c r="G385" s="0" t="inlineStr"/>
-      <c r="H385" s="0" t="inlineStr"/>
-      <c r="R385" s="0" t="inlineStr"/>
-      <c r="S385" s="0" t="inlineStr"/>
-      <c r="T385" s="0" t="inlineStr"/>
       <c r="U385" s="0" t="b">
         <v>0</v>
       </c>
@@ -26194,7 +25525,6 @@
           <t>LL1244</t>
         </is>
       </c>
-      <c r="R386" s="0" t="inlineStr"/>
       <c r="S386" s="0" t="inlineStr">
         <is>
           <t> ΔhfsB::kan</t>
@@ -26245,8 +25575,6 @@
           <t>LL1301</t>
         </is>
       </c>
-      <c r="L387" s="0" t="inlineStr"/>
-      <c r="R387" s="0" t="inlineStr"/>
       <c r="S387" s="0" t="inlineStr">
         <is>
           <t> ΔhfsB::kan</t>
@@ -26297,7 +25625,6 @@
           <t>LL1258</t>
         </is>
       </c>
-      <c r="R388" s="0" t="inlineStr"/>
       <c r="S388" s="0" t="inlineStr">
         <is>
           <t> ΔhfsB::kan</t>
@@ -26348,9 +25675,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="L389" s="0" t="inlineStr"/>
-      <c r="P389" s="0" t="inlineStr"/>
-      <c r="R389" s="0" t="inlineStr"/>
       <c r="S389" s="0" t="inlineStr">
         <is>
           <t> ΔhfsAB::kan</t>
@@ -26401,9 +25725,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="L390" s="0" t="inlineStr"/>
-      <c r="P390" s="0" t="inlineStr"/>
-      <c r="R390" s="0" t="inlineStr"/>
       <c r="S390" s="0" t="inlineStr">
         <is>
           <t> ΔhfsCD::kan</t>
@@ -26449,16 +25770,11 @@
           <t>Thermoanaerobacter ethanolicus ATCC 31550</t>
         </is>
       </c>
-      <c r="H391" s="0" t="inlineStr"/>
-      <c r="L391" s="0" t="inlineStr"/>
-      <c r="P391" s="0" t="inlineStr"/>
       <c r="R391" s="0" t="inlineStr">
         <is>
           <t>tdk deletion</t>
         </is>
       </c>
-      <c r="S391" s="0" t="inlineStr"/>
-      <c r="T391" s="0" t="inlineStr"/>
       <c r="U391" s="0" t="b">
         <v>0</v>
       </c>
@@ -26498,8 +25814,6 @@
           <t>LL1025</t>
         </is>
       </c>
-      <c r="L392" s="0" t="inlineStr"/>
-      <c r="P392" s="0" t="inlineStr"/>
       <c r="R392" s="0" t="inlineStr">
         <is>
           <t>ΔxynA::0705 erm</t>
@@ -26957,16 +26271,11 @@
           <t>LL1355</t>
         </is>
       </c>
-      <c r="I400" s="0" t="inlineStr"/>
-      <c r="L400" s="0" t="inlineStr"/>
-      <c r="N400" s="0" t="inlineStr"/>
-      <c r="P400" s="0" t="inlineStr"/>
       <c r="R400" s="0" t="inlineStr">
         <is>
           <t>Restreak of LL1355.  Resequenced by JGI.</t>
         </is>
       </c>
-      <c r="S400" s="0" t="inlineStr"/>
       <c r="T400" s="0" t="inlineStr">
         <is>
           <t>LL1355 _x000d_
@@ -27002,19 +26311,11 @@
           <t>*empty*</t>
         </is>
       </c>
-      <c r="G401" s="0" t="inlineStr"/>
-      <c r="H401" s="0" t="inlineStr"/>
-      <c r="I401" s="0" t="inlineStr"/>
-      <c r="L401" s="0" t="inlineStr"/>
-      <c r="N401" s="0" t="inlineStr"/>
-      <c r="P401" s="0" t="inlineStr"/>
       <c r="R401" s="0" t="inlineStr">
         <is>
           <t>Strain numbers LL1360-LL1366 were given out to 2 different people.  Since Chris's LL1360 was already sent for sequencing, we let Chris keep that number.  Everyone else got reassigned numbers.  LL1361-LL1366 strain IDs will not be used to avoid future confusion</t>
         </is>
       </c>
-      <c r="S401" s="0" t="inlineStr"/>
-      <c r="T401" s="0" t="inlineStr"/>
       <c r="U401" s="0" t="b">
         <v>0</v>
       </c>
@@ -27044,19 +26345,11 @@
           <t>*empty*</t>
         </is>
       </c>
-      <c r="G402" s="0" t="inlineStr"/>
-      <c r="H402" s="0" t="inlineStr"/>
-      <c r="I402" s="0" t="inlineStr"/>
-      <c r="L402" s="0" t="inlineStr"/>
-      <c r="N402" s="0" t="inlineStr"/>
-      <c r="P402" s="0" t="inlineStr"/>
       <c r="R402" s="0" t="inlineStr">
         <is>
           <t>Strain numbers LL1360-LL1366 were given out to 2 different people.  Since Chris's LL1360 was already sent for sequencing, we let Chris keep that number.  Everyone else got reassigned numbers.  LL1361-LL1366 strain IDs will not be used to avoid future confusion</t>
         </is>
       </c>
-      <c r="S402" s="0" t="inlineStr"/>
-      <c r="T402" s="0" t="inlineStr"/>
       <c r="U402" s="0" t="b">
         <v>0</v>
       </c>
@@ -27086,19 +26379,11 @@
           <t>*empty*</t>
         </is>
       </c>
-      <c r="G403" s="0" t="inlineStr"/>
-      <c r="H403" s="0" t="inlineStr"/>
-      <c r="I403" s="0" t="inlineStr"/>
-      <c r="L403" s="0" t="inlineStr"/>
-      <c r="N403" s="0" t="inlineStr"/>
-      <c r="P403" s="0" t="inlineStr"/>
       <c r="R403" s="0" t="inlineStr">
         <is>
           <t>Strain numbers LL1360-LL1366 were given out to 2 different people.  Since Chris's LL1360 was already sent for sequencing, we let Chris keep that number.  Everyone else got reassigned numbers.  LL1361-LL1366 strain IDs will not be used to avoid future confusion</t>
         </is>
       </c>
-      <c r="S403" s="0" t="inlineStr"/>
-      <c r="T403" s="0" t="inlineStr"/>
       <c r="U403" s="0" t="b">
         <v>0</v>
       </c>
@@ -27128,19 +26413,11 @@
           <t>*empty*</t>
         </is>
       </c>
-      <c r="G404" s="0" t="inlineStr"/>
-      <c r="H404" s="0" t="inlineStr"/>
-      <c r="I404" s="0" t="inlineStr"/>
-      <c r="L404" s="0" t="inlineStr"/>
-      <c r="N404" s="0" t="inlineStr"/>
-      <c r="P404" s="0" t="inlineStr"/>
       <c r="R404" s="0" t="inlineStr">
         <is>
           <t>Strain numbers LL1360-LL1366 were given out to 2 different people.  Since Chris's LL1360 was already sent for sequencing, we let Chris keep that number.  Everyone else got reassigned numbers.  LL1361-LL1366 strain IDs will not be used to avoid future confusion</t>
         </is>
       </c>
-      <c r="S404" s="0" t="inlineStr"/>
-      <c r="T404" s="0" t="inlineStr"/>
       <c r="U404" s="0" t="b">
         <v>0</v>
       </c>
@@ -27170,10 +26447,6 @@
           <t>*empty*</t>
         </is>
       </c>
-      <c r="G405" s="0" t="inlineStr"/>
-      <c r="I405" s="0" t="inlineStr"/>
-      <c r="L405" s="0" t="inlineStr"/>
-      <c r="N405" s="0" t="inlineStr"/>
       <c r="R405" s="0" t="inlineStr">
         <is>
           <t>Strain numbers LL1360-LL1366 were given out to 2 different people.  Since Chris's LL1360 was already sent for sequencing, we let Chris keep that number.  Everyone else got reassigned numbers.  LL1361-LL1366 strain IDs will not be used to avoid future confusion</t>
@@ -27182,8 +26455,6 @@
       <c r="U405" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W405" s="0" t="inlineStr"/>
-      <c r="X405" s="0" t="inlineStr"/>
       <c r="Y405" s="0" t="inlineStr">
         <is>
           <t>1365</t>
@@ -27210,10 +26481,6 @@
           <t>*empty*</t>
         </is>
       </c>
-      <c r="G406" s="0" t="inlineStr"/>
-      <c r="I406" s="0" t="inlineStr"/>
-      <c r="L406" s="0" t="inlineStr"/>
-      <c r="N406" s="0" t="inlineStr"/>
       <c r="R406" s="0" t="inlineStr">
         <is>
           <t>Strain numbers LL1360-LL1366 were given out to 2 different people.  Since Chris's LL1360 was already sent for sequencing, we let Chris keep that number.  Everyone else got reassigned numbers.  LL1361-LL1366 strain IDs will not be used to avoid future confusion</t>
@@ -27222,8 +26489,6 @@
       <c r="U406" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W406" s="0" t="inlineStr"/>
-      <c r="X406" s="0" t="inlineStr"/>
       <c r="Y406" s="0" t="inlineStr">
         <is>
           <t>1366</t>
@@ -27299,8 +26564,6 @@
       <c r="U407" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W407" s="0" t="inlineStr"/>
-      <c r="X407" s="0" t="inlineStr"/>
       <c r="Y407" s="0" t="inlineStr">
         <is>
           <t>1367</t>
@@ -27376,8 +26639,6 @@
       <c r="U408" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W408" s="0" t="inlineStr"/>
-      <c r="X408" s="0" t="inlineStr"/>
       <c r="Y408" s="0" t="inlineStr">
         <is>
           <t>1368</t>
@@ -27453,8 +26714,6 @@
       <c r="U409" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W409" s="0" t="inlineStr"/>
-      <c r="X409" s="0" t="inlineStr"/>
       <c r="Y409" s="0" t="inlineStr">
         <is>
           <t>1369</t>
@@ -27530,8 +26789,6 @@
       <c r="U410" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W410" s="0" t="inlineStr"/>
-      <c r="X410" s="0" t="inlineStr"/>
       <c r="Y410" s="0" t="inlineStr">
         <is>
           <t>1370</t>
@@ -27607,8 +26864,6 @@
       <c r="U411" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W411" s="0" t="inlineStr"/>
-      <c r="X411" s="0" t="inlineStr"/>
       <c r="Y411" s="0" t="inlineStr">
         <is>
           <t>1371</t>
@@ -27704,7 +26959,6 @@
           <t>Escherichia coli NEB C3013I</t>
         </is>
       </c>
-      <c r="H413" s="0" t="inlineStr"/>
       <c r="I413" s="0" t="inlineStr">
         <is>
           <t>pNT-AdhE*</t>
@@ -27720,14 +26974,11 @@
           <t>Carb100</t>
         </is>
       </c>
-      <c r="P413" s="0" t="inlineStr"/>
       <c r="R413" s="0" t="inlineStr">
         <is>
           <t>LL346 AdhE expression strain, his-tagged</t>
         </is>
       </c>
-      <c r="S413" s="0" t="inlineStr"/>
-      <c r="T413" s="0" t="inlineStr"/>
       <c r="U413" s="0" t="b">
         <v>0</v>
       </c>
@@ -27772,7 +27023,6 @@
           <t>Escherichia coli NEB C3013I</t>
         </is>
       </c>
-      <c r="H414" s="0" t="inlineStr"/>
       <c r="I414" s="0" t="inlineStr">
         <is>
           <t>pNT-E50C</t>
@@ -27788,14 +27038,11 @@
           <t>Carb100</t>
         </is>
       </c>
-      <c r="P414" s="0" t="inlineStr"/>
       <c r="R414" s="0" t="inlineStr">
         <is>
           <t>D494G AdhE expression strain, his-tagged</t>
         </is>
       </c>
-      <c r="S414" s="0" t="inlineStr"/>
-      <c r="T414" s="0" t="inlineStr"/>
       <c r="U414" s="0" t="b">
         <v>0</v>
       </c>
@@ -27840,7 +27087,6 @@
           <t>Escherichia coli NEB C3013I</t>
         </is>
       </c>
-      <c r="H415" s="0" t="inlineStr"/>
       <c r="I415" s="0" t="inlineStr">
         <is>
           <t>pNT-3</t>
@@ -27861,8 +27107,6 @@
           <t>LL1025 AdhE expression strain, his-tagged</t>
         </is>
       </c>
-      <c r="S415" s="0" t="inlineStr"/>
-      <c r="T415" s="0" t="inlineStr"/>
       <c r="U415" s="0" t="b">
         <v>0</v>
       </c>
@@ -27907,7 +27151,6 @@
           <t>Escherichia coli NEB C3013I</t>
         </is>
       </c>
-      <c r="H416" s="0" t="inlineStr"/>
       <c r="I416" s="0" t="inlineStr">
         <is>
           <t>pNT-1049</t>
@@ -27923,14 +27166,11 @@
           <t>Carb100</t>
         </is>
       </c>
-      <c r="P416" s="0" t="inlineStr"/>
       <c r="R416" s="0" t="inlineStr">
         <is>
           <t>LL1049 AdhE expression strain, his-tagged</t>
         </is>
       </c>
-      <c r="S416" s="0" t="inlineStr"/>
-      <c r="T416" s="0" t="inlineStr"/>
       <c r="U416" s="0" t="b">
         <v>0</v>
       </c>
@@ -27975,7 +27215,6 @@
           <t>Escherichia coli NEB C3013I</t>
         </is>
       </c>
-      <c r="H417" s="0" t="inlineStr"/>
       <c r="I417" s="0" t="inlineStr">
         <is>
           <t>pNT-1040</t>
@@ -27991,14 +27230,11 @@
           <t>Carb100</t>
         </is>
       </c>
-      <c r="P417" s="0" t="inlineStr"/>
       <c r="R417" s="0" t="inlineStr">
         <is>
           <t>LL1040 AdhE expression strain, his-tagged</t>
         </is>
       </c>
-      <c r="S417" s="0" t="inlineStr"/>
-      <c r="T417" s="0" t="inlineStr"/>
       <c r="U417" s="0" t="b">
         <v>0</v>
       </c>
@@ -28043,7 +27279,6 @@
           <t>Escherichia coli NEB C3013I</t>
         </is>
       </c>
-      <c r="H418" s="0" t="inlineStr"/>
       <c r="I418" s="0" t="inlineStr">
         <is>
           <t>pNT-CALML3</t>
@@ -28059,14 +27294,11 @@
           <t>Carb100</t>
         </is>
       </c>
-      <c r="P418" s="0" t="inlineStr"/>
       <c r="R418" s="0" t="inlineStr">
         <is>
           <t>control plasmid, his-tagged</t>
         </is>
       </c>
-      <c r="S418" s="0" t="inlineStr"/>
-      <c r="T418" s="0" t="inlineStr"/>
       <c r="U418" s="0" t="b">
         <v>0</v>
       </c>
@@ -28111,15 +27343,11 @@
           <t>Thermoanaerobacter ethanolicus ATCC 31550</t>
         </is>
       </c>
-      <c r="H419" s="0" t="inlineStr"/>
-      <c r="P419" s="0" t="inlineStr"/>
       <c r="R419" s="0" t="inlineStr">
         <is>
           <t>X11 from Xiongjun's collection.  T. ethanolicus with adhE, adhA and adhB deleted</t>
         </is>
       </c>
-      <c r="S419" s="0" t="inlineStr"/>
-      <c r="T419" s="0" t="inlineStr"/>
       <c r="U419" s="0" t="b">
         <v>0</v>
       </c>
@@ -28159,9 +27387,6 @@
           <t>LL1210</t>
         </is>
       </c>
-      <c r="I420" s="0" t="inlineStr"/>
-      <c r="L420" s="0" t="inlineStr"/>
-      <c r="N420" s="0" t="inlineStr"/>
       <c r="P420" s="0" t="inlineStr">
         <is>
           <t>Liang Tian notebook 2 p. 20-21</t>
@@ -28197,8 +27422,6 @@
       <c r="U420" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W420" s="0" t="inlineStr"/>
-      <c r="X420" s="0" t="inlineStr"/>
       <c r="Y420" s="0" t="inlineStr">
         <is>
           <t>1380</t>
@@ -28245,7 +27468,6 @@
           <t>CTFUD</t>
         </is>
       </c>
-      <c r="N421" s="0" t="inlineStr"/>
       <c r="P421" s="0" t="inlineStr">
         <is>
           <t>SH Book VIII Pg 88 –SH Book IX Pg 4</t>
@@ -28274,8 +27496,6 @@
       <c r="U421" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="W421" s="0" t="inlineStr"/>
-      <c r="X421" s="0" t="inlineStr"/>
       <c r="Y421" s="0" t="inlineStr">
         <is>
           <t>1381</t>
@@ -28312,8 +27532,6 @@
           <t>LL1318</t>
         </is>
       </c>
-      <c r="L422" s="0" t="inlineStr"/>
-      <c r="O422" s="1"/>
       <c r="R422" s="0" t="inlineStr">
         <is>
           <t>LL1318 Δkor::cat_x000d_
@@ -28378,9 +27596,6 @@
           <t>LL1305</t>
         </is>
       </c>
-      <c r="I423" s="0" t="inlineStr"/>
-      <c r="L423" s="0" t="inlineStr"/>
-      <c r="O423" s="1"/>
       <c r="P423" s="0" t="inlineStr">
         <is>
           <t>Lexie notebook 2 p. 98</t>
@@ -28442,9 +27657,6 @@
           <t>LL1273</t>
         </is>
       </c>
-      <c r="I424" s="0" t="inlineStr"/>
-      <c r="L424" s="0" t="inlineStr"/>
-      <c r="O424" s="1"/>
       <c r="P424" s="0" t="inlineStr">
         <is>
           <t>MB notebook #18 p. 44-50</t>
@@ -28507,9 +27719,6 @@
           <t>LL1277</t>
         </is>
       </c>
-      <c r="I425" s="0" t="inlineStr"/>
-      <c r="L425" s="0" t="inlineStr"/>
-      <c r="O425" s="1"/>
       <c r="P425" s="0" t="inlineStr">
         <is>
           <t>MB notebook #18 p. 44-50</t>
@@ -28574,9 +27783,6 @@
           <t>LL1328</t>
         </is>
       </c>
-      <c r="I426" s="0" t="inlineStr"/>
-      <c r="L426" s="0" t="inlineStr"/>
-      <c r="O426" s="1"/>
       <c r="P426" s="0" t="inlineStr">
         <is>
           <t>Lexie notebook #2, p. 98</t>
@@ -28812,7 +28018,6 @@
           <t>LL1070</t>
         </is>
       </c>
-      <c r="I429" s="0" t="inlineStr"/>
       <c r="L429" s="0" t="inlineStr">
         <is>
           <t>CTFUD</t>
@@ -29348,7 +28553,6 @@
       <c r="C437" s="0" t="b">
         <v>0</v>
       </c>
-      <c r="D437" s="0" t="inlineStr"/>
       <c r="E437" s="0" t="b">
         <v>0</v>
       </c>
@@ -29372,8 +28576,6 @@
           <t>pLT_54</t>
         </is>
       </c>
-      <c r="P437" s="0" t="inlineStr"/>
-      <c r="Q437" s="0" t="inlineStr"/>
       <c r="R437" s="0" t="inlineStr">
         <is>
           <t>LL1004 pLT_54 (adhA+PDC7)-2</t>
@@ -29598,7 +28800,6 @@
           <t>Mascoma strain M1673.  M795 with tdk deletion</t>
         </is>
       </c>
-      <c r="S441" s="0" t="inlineStr"/>
       <c r="T441" s="0" t="inlineStr">
         <is>
           <t>LL1400 _x000d_
@@ -29634,11 +28835,6 @@
           <t>Tianyong Zheng</t>
         </is>
       </c>
-      <c r="G442" s="0" t="inlineStr"/>
-      <c r="H442" s="0" t="inlineStr"/>
-      <c r="R442" s="0" t="inlineStr"/>
-      <c r="S442" s="0" t="inlineStr"/>
-      <c r="T442" s="0" t="inlineStr"/>
       <c r="U442" s="0" t="b">
         <v>0</v>
       </c>
@@ -29668,11 +28864,6 @@
           <t>Tianyong Zheng</t>
         </is>
       </c>
-      <c r="G443" s="0" t="inlineStr"/>
-      <c r="H443" s="0" t="inlineStr"/>
-      <c r="R443" s="0" t="inlineStr"/>
-      <c r="S443" s="0" t="inlineStr"/>
-      <c r="T443" s="0" t="inlineStr"/>
       <c r="U443" s="0" t="b">
         <v>0</v>
       </c>
@@ -29832,13 +29023,11 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="H446" s="0" t="inlineStr"/>
       <c r="R446" s="0" t="inlineStr">
         <is>
           <t>C. therm ∆cip::cipA*∆T2Doc (clone 617-1-2F2b-A1)</t>
         </is>
       </c>
-      <c r="T446" s="0" t="inlineStr"/>
       <c r="U446" s="0" t="b">
         <v>0</v>
       </c>
@@ -29973,8 +29162,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="P449" s="0" t="inlineStr"/>
-      <c r="Q449" s="0" t="inlineStr"/>
       <c r="R449" s="0" t="inlineStr">
         <is>
           <t>C. therm ∆hydG (clone 758-3-1-2s)</t>
@@ -30031,8 +29218,6 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="P450" s="0" t="inlineStr"/>
-      <c r="Q450" s="0" t="inlineStr"/>
       <c r="R450" s="0" t="inlineStr">
         <is>
           <t>C. therm ∆pfl (clone 803-1-1-1)</t>
@@ -30089,14 +29274,11 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="P451" s="0" t="inlineStr"/>
-      <c r="Q451" s="0" t="inlineStr"/>
       <c r="R451" s="0" t="inlineStr">
         <is>
           <t>C. therm ∆pfl (clone 804-2-1-1)</t>
         </is>
       </c>
-      <c r="S451" s="0" t="inlineStr"/>
       <c r="T451" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -30143,14 +29325,11 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="P452" s="0" t="inlineStr"/>
-      <c r="Q452" s="0" t="inlineStr"/>
       <c r="R452" s="0" t="inlineStr">
         <is>
           <t>C. therm ∆pfl (clone 804-2-2-1)</t>
         </is>
       </c>
-      <c r="S452" s="0" t="inlineStr"/>
       <c r="T452" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -30197,14 +29376,11 @@
           <t>LL345</t>
         </is>
       </c>
-      <c r="P453" s="0" t="inlineStr"/>
-      <c r="Q453" s="0" t="inlineStr"/>
       <c r="R453" s="0" t="inlineStr">
         <is>
           <t>C. therm ∆pfl (clone 804-2-3-1)</t>
         </is>
       </c>
-      <c r="S453" s="0" t="inlineStr"/>
       <c r="T453" s="0" t="inlineStr">
         <is>
           <t>LL345  ∆hpt_x000d_
@@ -31208,7 +30384,6 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="Q475" s="0" t="inlineStr"/>
       <c r="R475" s="0" t="inlineStr">
         <is>
           <t>M10, or putative betaxylosidase 1447</t>
@@ -31248,14 +30423,11 @@
           <t>Thermoanaerobacterium saccharolyticum</t>
         </is>
       </c>
-      <c r="H476" s="0" t="inlineStr"/>
       <c r="R476" s="0" t="inlineStr">
         <is>
           <t>M11, Xyn A + Xyn B</t>
         </is>
       </c>
-      <c r="S476" s="0" t="inlineStr"/>
-      <c r="T476" s="0" t="inlineStr"/>
       <c r="U476" s="0" t="b">
         <v>0</v>
       </c>
@@ -31588,7 +30760,6 @@
           <t>Clostridium clariflavium</t>
         </is>
       </c>
-      <c r="Q484" s="0" t="inlineStr"/>
       <c r="R484" s="0" t="inlineStr">
         <is>
           <t>DSM 19732. Marybeth grew this strain in CTFUD medium, pH 7 at 55C on 3-18-2015.</t>
@@ -31628,7 +30799,6 @@
           <t>Clostridium clariflavium</t>
         </is>
       </c>
-      <c r="Q485" s="0" t="inlineStr"/>
       <c r="R485" s="0" t="inlineStr">
         <is>
           <t>strain 42A</t>
@@ -31707,7 +30877,6 @@
           <t>Clostridium clariflavium</t>
         </is>
       </c>
-      <c r="Q487" s="0" t="inlineStr"/>
       <c r="R487" s="0" t="inlineStr">
         <is>
           <t>strain SA115</t>
@@ -31747,13 +30916,11 @@
           <t>Clostridium straminosolvens</t>
         </is>
       </c>
-      <c r="H488" s="0" t="inlineStr"/>
       <c r="R488" s="0" t="inlineStr">
         <is>
           <t>Strain CSK1, DSM 16021.  Marybeth grew this strain in CTFUD medium, pH 7 at 50C and 55C on 3-18-2015.</t>
         </is>
       </c>
-      <c r="T488" s="0" t="inlineStr"/>
       <c r="U488" s="0" t="b">
         <v>0</v>
       </c>
@@ -31788,13 +30955,11 @@
           <t>Clostridium clariflavium</t>
         </is>
       </c>
-      <c r="H489" s="0" t="inlineStr"/>
       <c r="R489" s="0" t="inlineStr">
         <is>
           <t>strain SA1 (OLD)</t>
         </is>
       </c>
-      <c r="T489" s="0" t="inlineStr"/>
       <c r="U489" s="0" t="b">
         <v>0</v>
       </c>
@@ -31829,13 +30994,11 @@
           <t>Clostridium cellulolyticum</t>
         </is>
       </c>
-      <c r="H490" s="0" t="inlineStr"/>
       <c r="R490" s="0" t="inlineStr">
         <is>
           <t>C. cellulolyticum</t>
         </is>
       </c>
-      <c r="T490" s="0" t="inlineStr"/>
       <c r="U490" s="0" t="b">
         <v>0</v>
       </c>
@@ -31870,7 +31033,6 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="H491" s="0" t="inlineStr"/>
       <c r="Q491" s="0" t="inlineStr">
         <is>
           <t>M0525</t>
@@ -31881,7 +31043,6 @@
           <t>strain MO525 (Mascoma)</t>
         </is>
       </c>
-      <c r="T491" s="0" t="inlineStr"/>
       <c r="U491" s="0" t="b">
         <v>0</v>
       </c>
@@ -31916,7 +31077,6 @@
           <t>Clostridium thermocellum</t>
         </is>
       </c>
-      <c r="I492" s="0" t="inlineStr"/>
       <c r="Q492" s="0" t="inlineStr">
         <is>
           <t>M0526</t>

</xml_diff>